<commit_message>
Maj JDT Lopez Jimmy + maquette
Mise à jour du journal de travail et de la maquette
</commit_message>
<xml_diff>
--- a/Doc/DemoMotJDT-Lopezji.xlsx
+++ b/Doc/DemoMotJDT-Lopezji.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="78">
   <si>
     <t>Module :</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Création de mes maquettes personnelles. Je fais sur paint un schéma de comment je voudrais que le site soit mis en place. Je structure la page de profile et la page d'accueil. Une fois les deux schémas terminés, je compare mes exemples avec ceux de Fabien et nous convenons d'une version finale pour les maquettes.</t>
+  </si>
+  <si>
+    <t>Design site</t>
+  </si>
+  <si>
+    <t>J'ai crée le logo du site avec son nom et le background est en cours de création. Si ça prend autant de temps c'est car je dois prendre des images contenant un personnage de jeu et le détourer pour extraire uniquement le personnage important. Je le place ensuite sur le background de manière organisée. Le but est d'avoir un background réunissant beaucoup de personnages de jeux connus. J'ai fait deux rangées pour commencer et comme cela prend beaucoup de temps nous le gardons comme ça pour le moment ce qui nous permet déjà de voir à quoi ressemblera le site. Le background sera terminé quand les tâches les plus importantes seront terminées.</t>
   </si>
 </sst>
 </file>
@@ -2095,8 +2101,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2578,7 +2584,9 @@
       <c r="B37" s="66">
         <v>17</v>
       </c>
-      <c r="C37" s="28"/>
+      <c r="C37" s="28" t="s">
+        <v>76</v>
+      </c>
       <c r="D37" s="37"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
@@ -20504,8 +20512,8 @@
   </sheetPr>
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21085,27 +21093,51 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="13"/>
+      <c r="A52" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="8">
+        <v>15</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="14"/>
+      <c r="A53" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="6">
+        <v>1</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="14"/>
+    <row r="54" spans="1:4" ht="108" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="6">
+        <v>10</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="14"/>
+      <c r="A55" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="6">
+        <v>1</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21180,7 +21212,7 @@
       </c>
       <c r="B67" s="76">
         <f>SUM(B52:B66)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
MAJ JDT JLZ + TYPO3
Mise à jour du journal de travail et supression du dossier typo3
</commit_message>
<xml_diff>
--- a/Doc/DemoMotJDT-Lopezji.xlsx
+++ b/Doc/DemoMotJDT-Lopezji.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="83">
   <si>
     <t>Module :</t>
   </si>
@@ -294,6 +294,21 @@
   </si>
   <si>
     <t>J'ai crée le logo du site avec son nom et le background est en cours de création. Si ça prend autant de temps c'est car je dois prendre des images contenant un personnage de jeu et le détourer pour extraire uniquement le personnage important. Je le place ensuite sur le background de manière organisée. Le but est d'avoir un background réunissant beaucoup de personnages de jeux connus. J'ai fait deux rangées pour commencer et comme cela prend beaucoup de temps nous le gardons comme ça pour le moment ce qui nous permet déjà de voir à quoi ressemblera le site. Le background sera terminé quand les tâches les plus importantes seront terminées.</t>
+  </si>
+  <si>
+    <t>Recherche d'une manière d'avoir le site sur git afin de modifier du contenu ensemble sans gêner l'autre en évitant de stocker les fichier que l'on ne modifie pas pour eviter de surcharger le répertoire.  M. Gruaz nous a montré que l'on peut faire des .gitignore pour que git ignore certains fichier que l'on nomme dans ce document afin de ne pas les traiter. Nous avons aussi créé de nouvelles branches afin de commencer les commit avec les mêmes documents.</t>
+  </si>
+  <si>
+    <t>Exportation de jeux flash</t>
+  </si>
+  <si>
+    <t>J'ai montré à Fabien comment exporter des jeux en format SWF afin qu'il puisse préparer plusieurs jeux pour le site</t>
+  </si>
+  <si>
+    <t>Mise à jour du journal de travail + Commit de gitkraken</t>
+  </si>
+  <si>
+    <t>J'ai chercher comment installer une extension permettant d'écrire du code PHP directement sur typo3. J'ai installé plusieurs extension mais elle ne fonctionnent malheureusement pas avec notre version de typo3. J'ai donc continué à chercher des solutions. J'ai suivi un tutoriel qui montre comment créer un script en php qu'il faudra appeler pour que le code écrit à l'intérieur s'execute mais cela ne fonctionne pas non plus. J'ai continué à chercher des extension et une des extension que j'ai installé a créé une erreur qui rendait l'interface typo3 inutilisable. une erreur apparaissait et ne laissait rien faire. J'ai donc chercher comment désinstaller une extension sans l'interface (donc avec les fichiers) et j'ai trouvé. Il fallait chercher dans le fichier PackageStates.php et mettre en commentaire la dernièrer extension que j'ai installé, ensuite l'interface s'est lancée comme il faut et j'ai désinstallé l'extension. Nous sommes allé chercher Mme hardegger mais nous ne l'avons pas trouvé. En attendant, j'ai continué à faire le background du site en prenant des personnages et en les détourant. Nous avons ensuite trouvé Mme hardegger et elle nous a expliqué qu'il fallait tout simplement créer une extension non pas pour écrire en php mais pour directement effectuer ce que l'on voulait coder en php (donc une extension qui gère les jeux flashs). J'ai regardé un tutoriel et j'ai installé l'extension "extension builder" qui sert à créer des extensions. J'ai vu un peu comment l'extension fonctionne et je vais pouvoir m'y mettre dès la prochaine fois.</t>
   </si>
 </sst>
 </file>
@@ -1383,6 +1398,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1391,12 +1412,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -2101,8 +2116,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2603,7 +2618,9 @@
       <c r="B38" s="67">
         <v>18</v>
       </c>
-      <c r="C38" s="28"/>
+      <c r="C38" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
@@ -3166,27 +3183,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3216,27 +3233,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3274,470 +3291,470 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="110" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="114"/>
+      <c r="AE2" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="111"/>
-      <c r="AG2" s="111"/>
-      <c r="AH2" s="111"/>
-      <c r="AI2" s="111"/>
-      <c r="AJ2" s="111"/>
-      <c r="AK2" s="111"/>
-      <c r="AL2" s="111"/>
-      <c r="AM2" s="111"/>
-      <c r="AN2" s="111"/>
-      <c r="AO2" s="111"/>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="111"/>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AU2" s="111"/>
-      <c r="AV2" s="111"/>
-      <c r="AW2" s="111"/>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="111"/>
-      <c r="AZ2" s="111"/>
-      <c r="BA2" s="111"/>
-      <c r="BB2" s="111"/>
-      <c r="BC2" s="111"/>
-      <c r="BD2" s="111"/>
-      <c r="BE2" s="112"/>
-      <c r="BF2" s="110" t="s">
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AH2" s="113"/>
+      <c r="AI2" s="113"/>
+      <c r="AJ2" s="113"/>
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="113"/>
+      <c r="AO2" s="113"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="113"/>
+      <c r="AR2" s="113"/>
+      <c r="AS2" s="113"/>
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BD2" s="113"/>
+      <c r="BE2" s="114"/>
+      <c r="BF2" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="BG2" s="111"/>
-      <c r="BH2" s="111"/>
-      <c r="BI2" s="111"/>
-      <c r="BJ2" s="111"/>
-      <c r="BK2" s="111"/>
-      <c r="BL2" s="111"/>
-      <c r="BM2" s="111"/>
-      <c r="BN2" s="111"/>
-      <c r="BO2" s="111"/>
-      <c r="BP2" s="111"/>
-      <c r="BQ2" s="111"/>
-      <c r="BR2" s="111"/>
-      <c r="BS2" s="111"/>
-      <c r="BT2" s="111"/>
-      <c r="BU2" s="111"/>
-      <c r="BV2" s="111"/>
-      <c r="BW2" s="111"/>
-      <c r="BX2" s="111"/>
-      <c r="BY2" s="111"/>
-      <c r="BZ2" s="111"/>
-      <c r="CA2" s="111"/>
-      <c r="CB2" s="111"/>
-      <c r="CC2" s="111"/>
-      <c r="CD2" s="111"/>
-      <c r="CE2" s="111"/>
-      <c r="CF2" s="112"/>
-      <c r="CG2" s="110" t="s">
+      <c r="BG2" s="113"/>
+      <c r="BH2" s="113"/>
+      <c r="BI2" s="113"/>
+      <c r="BJ2" s="113"/>
+      <c r="BK2" s="113"/>
+      <c r="BL2" s="113"/>
+      <c r="BM2" s="113"/>
+      <c r="BN2" s="113"/>
+      <c r="BO2" s="113"/>
+      <c r="BP2" s="113"/>
+      <c r="BQ2" s="113"/>
+      <c r="BR2" s="113"/>
+      <c r="BS2" s="113"/>
+      <c r="BT2" s="113"/>
+      <c r="BU2" s="113"/>
+      <c r="BV2" s="113"/>
+      <c r="BW2" s="113"/>
+      <c r="BX2" s="113"/>
+      <c r="BY2" s="113"/>
+      <c r="BZ2" s="113"/>
+      <c r="CA2" s="113"/>
+      <c r="CB2" s="113"/>
+      <c r="CC2" s="113"/>
+      <c r="CD2" s="113"/>
+      <c r="CE2" s="113"/>
+      <c r="CF2" s="114"/>
+      <c r="CG2" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="CH2" s="111"/>
-      <c r="CI2" s="111"/>
-      <c r="CJ2" s="111"/>
-      <c r="CK2" s="111"/>
-      <c r="CL2" s="111"/>
-      <c r="CM2" s="111"/>
-      <c r="CN2" s="111"/>
-      <c r="CO2" s="111"/>
-      <c r="CP2" s="111"/>
-      <c r="CQ2" s="111"/>
-      <c r="CR2" s="111"/>
-      <c r="CS2" s="111"/>
-      <c r="CT2" s="111"/>
-      <c r="CU2" s="111"/>
-      <c r="CV2" s="111"/>
-      <c r="CW2" s="111"/>
-      <c r="CX2" s="111"/>
-      <c r="CY2" s="111"/>
-      <c r="CZ2" s="111"/>
-      <c r="DA2" s="111"/>
-      <c r="DB2" s="111"/>
-      <c r="DC2" s="111"/>
-      <c r="DD2" s="111"/>
-      <c r="DE2" s="111"/>
-      <c r="DF2" s="111"/>
-      <c r="DG2" s="112"/>
-      <c r="DH2" s="110" t="s">
+      <c r="CH2" s="113"/>
+      <c r="CI2" s="113"/>
+      <c r="CJ2" s="113"/>
+      <c r="CK2" s="113"/>
+      <c r="CL2" s="113"/>
+      <c r="CM2" s="113"/>
+      <c r="CN2" s="113"/>
+      <c r="CO2" s="113"/>
+      <c r="CP2" s="113"/>
+      <c r="CQ2" s="113"/>
+      <c r="CR2" s="113"/>
+      <c r="CS2" s="113"/>
+      <c r="CT2" s="113"/>
+      <c r="CU2" s="113"/>
+      <c r="CV2" s="113"/>
+      <c r="CW2" s="113"/>
+      <c r="CX2" s="113"/>
+      <c r="CY2" s="113"/>
+      <c r="CZ2" s="113"/>
+      <c r="DA2" s="113"/>
+      <c r="DB2" s="113"/>
+      <c r="DC2" s="113"/>
+      <c r="DD2" s="113"/>
+      <c r="DE2" s="113"/>
+      <c r="DF2" s="113"/>
+      <c r="DG2" s="114"/>
+      <c r="DH2" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="DI2" s="111"/>
-      <c r="DJ2" s="111"/>
-      <c r="DK2" s="111"/>
-      <c r="DL2" s="111"/>
-      <c r="DM2" s="111"/>
-      <c r="DN2" s="111"/>
-      <c r="DO2" s="111"/>
-      <c r="DP2" s="111"/>
-      <c r="DQ2" s="111"/>
-      <c r="DR2" s="111"/>
-      <c r="DS2" s="111"/>
-      <c r="DT2" s="111"/>
-      <c r="DU2" s="111"/>
-      <c r="DV2" s="111"/>
-      <c r="DW2" s="111"/>
-      <c r="DX2" s="111"/>
-      <c r="DY2" s="111"/>
-      <c r="DZ2" s="111"/>
-      <c r="EA2" s="111"/>
-      <c r="EB2" s="111"/>
-      <c r="EC2" s="111"/>
-      <c r="ED2" s="111"/>
-      <c r="EE2" s="111"/>
-      <c r="EF2" s="111"/>
-      <c r="EG2" s="111"/>
-      <c r="EH2" s="112"/>
-      <c r="EI2" s="110" t="s">
+      <c r="DI2" s="113"/>
+      <c r="DJ2" s="113"/>
+      <c r="DK2" s="113"/>
+      <c r="DL2" s="113"/>
+      <c r="DM2" s="113"/>
+      <c r="DN2" s="113"/>
+      <c r="DO2" s="113"/>
+      <c r="DP2" s="113"/>
+      <c r="DQ2" s="113"/>
+      <c r="DR2" s="113"/>
+      <c r="DS2" s="113"/>
+      <c r="DT2" s="113"/>
+      <c r="DU2" s="113"/>
+      <c r="DV2" s="113"/>
+      <c r="DW2" s="113"/>
+      <c r="DX2" s="113"/>
+      <c r="DY2" s="113"/>
+      <c r="DZ2" s="113"/>
+      <c r="EA2" s="113"/>
+      <c r="EB2" s="113"/>
+      <c r="EC2" s="113"/>
+      <c r="ED2" s="113"/>
+      <c r="EE2" s="113"/>
+      <c r="EF2" s="113"/>
+      <c r="EG2" s="113"/>
+      <c r="EH2" s="114"/>
+      <c r="EI2" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="111"/>
-      <c r="EK2" s="111"/>
-      <c r="EL2" s="111"/>
-      <c r="EM2" s="111"/>
-      <c r="EN2" s="111"/>
-      <c r="EO2" s="111"/>
-      <c r="EP2" s="111"/>
-      <c r="EQ2" s="111"/>
-      <c r="ER2" s="111"/>
-      <c r="ES2" s="111"/>
-      <c r="ET2" s="111"/>
-      <c r="EU2" s="111"/>
-      <c r="EV2" s="111"/>
-      <c r="EW2" s="111"/>
-      <c r="EX2" s="111"/>
-      <c r="EY2" s="111"/>
-      <c r="EZ2" s="111"/>
-      <c r="FA2" s="111"/>
-      <c r="FB2" s="111"/>
-      <c r="FC2" s="111"/>
-      <c r="FD2" s="111"/>
-      <c r="FE2" s="111"/>
-      <c r="FF2" s="111"/>
-      <c r="FG2" s="111"/>
-      <c r="FH2" s="111"/>
-      <c r="FI2" s="112"/>
-      <c r="FJ2" s="110" t="s">
+      <c r="EJ2" s="113"/>
+      <c r="EK2" s="113"/>
+      <c r="EL2" s="113"/>
+      <c r="EM2" s="113"/>
+      <c r="EN2" s="113"/>
+      <c r="EO2" s="113"/>
+      <c r="EP2" s="113"/>
+      <c r="EQ2" s="113"/>
+      <c r="ER2" s="113"/>
+      <c r="ES2" s="113"/>
+      <c r="ET2" s="113"/>
+      <c r="EU2" s="113"/>
+      <c r="EV2" s="113"/>
+      <c r="EW2" s="113"/>
+      <c r="EX2" s="113"/>
+      <c r="EY2" s="113"/>
+      <c r="EZ2" s="113"/>
+      <c r="FA2" s="113"/>
+      <c r="FB2" s="113"/>
+      <c r="FC2" s="113"/>
+      <c r="FD2" s="113"/>
+      <c r="FE2" s="113"/>
+      <c r="FF2" s="113"/>
+      <c r="FG2" s="113"/>
+      <c r="FH2" s="113"/>
+      <c r="FI2" s="114"/>
+      <c r="FJ2" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="FK2" s="111"/>
-      <c r="FL2" s="111"/>
-      <c r="FM2" s="111"/>
-      <c r="FN2" s="111"/>
-      <c r="FO2" s="111"/>
-      <c r="FP2" s="111"/>
-      <c r="FQ2" s="111"/>
-      <c r="FR2" s="111"/>
-      <c r="FS2" s="111"/>
-      <c r="FT2" s="111"/>
-      <c r="FU2" s="111"/>
-      <c r="FV2" s="111"/>
-      <c r="FW2" s="111"/>
-      <c r="FX2" s="111"/>
-      <c r="FY2" s="111"/>
-      <c r="FZ2" s="111"/>
-      <c r="GA2" s="111"/>
-      <c r="GB2" s="111"/>
-      <c r="GC2" s="111"/>
-      <c r="GD2" s="111"/>
-      <c r="GE2" s="111"/>
-      <c r="GF2" s="111"/>
-      <c r="GG2" s="111"/>
-      <c r="GH2" s="111"/>
-      <c r="GI2" s="111"/>
-      <c r="GJ2" s="112"/>
-      <c r="GK2" s="110" t="s">
+      <c r="FK2" s="113"/>
+      <c r="FL2" s="113"/>
+      <c r="FM2" s="113"/>
+      <c r="FN2" s="113"/>
+      <c r="FO2" s="113"/>
+      <c r="FP2" s="113"/>
+      <c r="FQ2" s="113"/>
+      <c r="FR2" s="113"/>
+      <c r="FS2" s="113"/>
+      <c r="FT2" s="113"/>
+      <c r="FU2" s="113"/>
+      <c r="FV2" s="113"/>
+      <c r="FW2" s="113"/>
+      <c r="FX2" s="113"/>
+      <c r="FY2" s="113"/>
+      <c r="FZ2" s="113"/>
+      <c r="GA2" s="113"/>
+      <c r="GB2" s="113"/>
+      <c r="GC2" s="113"/>
+      <c r="GD2" s="113"/>
+      <c r="GE2" s="113"/>
+      <c r="GF2" s="113"/>
+      <c r="GG2" s="113"/>
+      <c r="GH2" s="113"/>
+      <c r="GI2" s="113"/>
+      <c r="GJ2" s="114"/>
+      <c r="GK2" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="GL2" s="111"/>
-      <c r="GM2" s="111"/>
-      <c r="GN2" s="111"/>
-      <c r="GO2" s="111"/>
-      <c r="GP2" s="111"/>
-      <c r="GQ2" s="111"/>
-      <c r="GR2" s="111"/>
-      <c r="GS2" s="111"/>
-      <c r="GT2" s="111"/>
-      <c r="GU2" s="111"/>
-      <c r="GV2" s="111"/>
-      <c r="GW2" s="111"/>
-      <c r="GX2" s="111"/>
-      <c r="GY2" s="111"/>
-      <c r="GZ2" s="111"/>
-      <c r="HA2" s="111"/>
-      <c r="HB2" s="111"/>
-      <c r="HC2" s="111"/>
-      <c r="HD2" s="111"/>
-      <c r="HE2" s="111"/>
-      <c r="HF2" s="111"/>
-      <c r="HG2" s="111"/>
-      <c r="HH2" s="111"/>
-      <c r="HI2" s="111"/>
-      <c r="HJ2" s="111"/>
-      <c r="HK2" s="112"/>
-      <c r="HL2" s="110" t="s">
+      <c r="GL2" s="113"/>
+      <c r="GM2" s="113"/>
+      <c r="GN2" s="113"/>
+      <c r="GO2" s="113"/>
+      <c r="GP2" s="113"/>
+      <c r="GQ2" s="113"/>
+      <c r="GR2" s="113"/>
+      <c r="GS2" s="113"/>
+      <c r="GT2" s="113"/>
+      <c r="GU2" s="113"/>
+      <c r="GV2" s="113"/>
+      <c r="GW2" s="113"/>
+      <c r="GX2" s="113"/>
+      <c r="GY2" s="113"/>
+      <c r="GZ2" s="113"/>
+      <c r="HA2" s="113"/>
+      <c r="HB2" s="113"/>
+      <c r="HC2" s="113"/>
+      <c r="HD2" s="113"/>
+      <c r="HE2" s="113"/>
+      <c r="HF2" s="113"/>
+      <c r="HG2" s="113"/>
+      <c r="HH2" s="113"/>
+      <c r="HI2" s="113"/>
+      <c r="HJ2" s="113"/>
+      <c r="HK2" s="114"/>
+      <c r="HL2" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="HM2" s="111"/>
-      <c r="HN2" s="111"/>
-      <c r="HO2" s="111"/>
-      <c r="HP2" s="111"/>
-      <c r="HQ2" s="111"/>
-      <c r="HR2" s="111"/>
-      <c r="HS2" s="111"/>
-      <c r="HT2" s="111"/>
-      <c r="HU2" s="111"/>
-      <c r="HV2" s="111"/>
-      <c r="HW2" s="111"/>
-      <c r="HX2" s="111"/>
-      <c r="HY2" s="111"/>
-      <c r="HZ2" s="111"/>
-      <c r="IA2" s="111"/>
-      <c r="IB2" s="111"/>
-      <c r="IC2" s="111"/>
-      <c r="ID2" s="111"/>
-      <c r="IE2" s="111"/>
-      <c r="IF2" s="111"/>
-      <c r="IG2" s="111"/>
-      <c r="IH2" s="111"/>
-      <c r="II2" s="111"/>
-      <c r="IJ2" s="111"/>
-      <c r="IK2" s="111"/>
-      <c r="IL2" s="112"/>
-      <c r="IM2" s="110" t="s">
+      <c r="HM2" s="113"/>
+      <c r="HN2" s="113"/>
+      <c r="HO2" s="113"/>
+      <c r="HP2" s="113"/>
+      <c r="HQ2" s="113"/>
+      <c r="HR2" s="113"/>
+      <c r="HS2" s="113"/>
+      <c r="HT2" s="113"/>
+      <c r="HU2" s="113"/>
+      <c r="HV2" s="113"/>
+      <c r="HW2" s="113"/>
+      <c r="HX2" s="113"/>
+      <c r="HY2" s="113"/>
+      <c r="HZ2" s="113"/>
+      <c r="IA2" s="113"/>
+      <c r="IB2" s="113"/>
+      <c r="IC2" s="113"/>
+      <c r="ID2" s="113"/>
+      <c r="IE2" s="113"/>
+      <c r="IF2" s="113"/>
+      <c r="IG2" s="113"/>
+      <c r="IH2" s="113"/>
+      <c r="II2" s="113"/>
+      <c r="IJ2" s="113"/>
+      <c r="IK2" s="113"/>
+      <c r="IL2" s="114"/>
+      <c r="IM2" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="IN2" s="111"/>
-      <c r="IO2" s="111"/>
-      <c r="IP2" s="111"/>
-      <c r="IQ2" s="111"/>
-      <c r="IR2" s="111"/>
-      <c r="IS2" s="111"/>
-      <c r="IT2" s="111"/>
-      <c r="IU2" s="111"/>
-      <c r="IV2" s="111"/>
-      <c r="IW2" s="111"/>
-      <c r="IX2" s="111"/>
-      <c r="IY2" s="111"/>
-      <c r="IZ2" s="111"/>
-      <c r="JA2" s="111"/>
-      <c r="JB2" s="111"/>
-      <c r="JC2" s="111"/>
-      <c r="JD2" s="111"/>
-      <c r="JE2" s="111"/>
-      <c r="JF2" s="111"/>
-      <c r="JG2" s="111"/>
-      <c r="JH2" s="111"/>
-      <c r="JI2" s="111"/>
-      <c r="JJ2" s="111"/>
-      <c r="JK2" s="111"/>
-      <c r="JL2" s="111"/>
-      <c r="JM2" s="112"/>
-      <c r="JN2" s="110" t="s">
+      <c r="IN2" s="113"/>
+      <c r="IO2" s="113"/>
+      <c r="IP2" s="113"/>
+      <c r="IQ2" s="113"/>
+      <c r="IR2" s="113"/>
+      <c r="IS2" s="113"/>
+      <c r="IT2" s="113"/>
+      <c r="IU2" s="113"/>
+      <c r="IV2" s="113"/>
+      <c r="IW2" s="113"/>
+      <c r="IX2" s="113"/>
+      <c r="IY2" s="113"/>
+      <c r="IZ2" s="113"/>
+      <c r="JA2" s="113"/>
+      <c r="JB2" s="113"/>
+      <c r="JC2" s="113"/>
+      <c r="JD2" s="113"/>
+      <c r="JE2" s="113"/>
+      <c r="JF2" s="113"/>
+      <c r="JG2" s="113"/>
+      <c r="JH2" s="113"/>
+      <c r="JI2" s="113"/>
+      <c r="JJ2" s="113"/>
+      <c r="JK2" s="113"/>
+      <c r="JL2" s="113"/>
+      <c r="JM2" s="114"/>
+      <c r="JN2" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="JO2" s="111"/>
-      <c r="JP2" s="111"/>
-      <c r="JQ2" s="111"/>
-      <c r="JR2" s="111"/>
-      <c r="JS2" s="111"/>
-      <c r="JT2" s="111"/>
-      <c r="JU2" s="111"/>
-      <c r="JV2" s="111"/>
-      <c r="JW2" s="111"/>
-      <c r="JX2" s="111"/>
-      <c r="JY2" s="111"/>
-      <c r="JZ2" s="111"/>
-      <c r="KA2" s="111"/>
-      <c r="KB2" s="111"/>
-      <c r="KC2" s="111"/>
-      <c r="KD2" s="111"/>
-      <c r="KE2" s="111"/>
-      <c r="KF2" s="111"/>
-      <c r="KG2" s="111"/>
-      <c r="KH2" s="111"/>
-      <c r="KI2" s="111"/>
-      <c r="KJ2" s="111"/>
-      <c r="KK2" s="111"/>
-      <c r="KL2" s="111"/>
-      <c r="KM2" s="111"/>
-      <c r="KN2" s="112"/>
-      <c r="KO2" s="110" t="s">
+      <c r="JO2" s="113"/>
+      <c r="JP2" s="113"/>
+      <c r="JQ2" s="113"/>
+      <c r="JR2" s="113"/>
+      <c r="JS2" s="113"/>
+      <c r="JT2" s="113"/>
+      <c r="JU2" s="113"/>
+      <c r="JV2" s="113"/>
+      <c r="JW2" s="113"/>
+      <c r="JX2" s="113"/>
+      <c r="JY2" s="113"/>
+      <c r="JZ2" s="113"/>
+      <c r="KA2" s="113"/>
+      <c r="KB2" s="113"/>
+      <c r="KC2" s="113"/>
+      <c r="KD2" s="113"/>
+      <c r="KE2" s="113"/>
+      <c r="KF2" s="113"/>
+      <c r="KG2" s="113"/>
+      <c r="KH2" s="113"/>
+      <c r="KI2" s="113"/>
+      <c r="KJ2" s="113"/>
+      <c r="KK2" s="113"/>
+      <c r="KL2" s="113"/>
+      <c r="KM2" s="113"/>
+      <c r="KN2" s="114"/>
+      <c r="KO2" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="KP2" s="111"/>
-      <c r="KQ2" s="111"/>
-      <c r="KR2" s="111"/>
-      <c r="KS2" s="111"/>
-      <c r="KT2" s="111"/>
-      <c r="KU2" s="111"/>
-      <c r="KV2" s="111"/>
-      <c r="KW2" s="111"/>
-      <c r="KX2" s="111"/>
-      <c r="KY2" s="111"/>
-      <c r="KZ2" s="111"/>
-      <c r="LA2" s="111"/>
-      <c r="LB2" s="111"/>
-      <c r="LC2" s="111"/>
-      <c r="LD2" s="111"/>
-      <c r="LE2" s="111"/>
-      <c r="LF2" s="111"/>
-      <c r="LG2" s="111"/>
-      <c r="LH2" s="111"/>
-      <c r="LI2" s="111"/>
-      <c r="LJ2" s="111"/>
-      <c r="LK2" s="111"/>
-      <c r="LL2" s="111"/>
-      <c r="LM2" s="111"/>
-      <c r="LN2" s="111"/>
-      <c r="LO2" s="112"/>
-      <c r="LP2" s="110" t="s">
+      <c r="KP2" s="113"/>
+      <c r="KQ2" s="113"/>
+      <c r="KR2" s="113"/>
+      <c r="KS2" s="113"/>
+      <c r="KT2" s="113"/>
+      <c r="KU2" s="113"/>
+      <c r="KV2" s="113"/>
+      <c r="KW2" s="113"/>
+      <c r="KX2" s="113"/>
+      <c r="KY2" s="113"/>
+      <c r="KZ2" s="113"/>
+      <c r="LA2" s="113"/>
+      <c r="LB2" s="113"/>
+      <c r="LC2" s="113"/>
+      <c r="LD2" s="113"/>
+      <c r="LE2" s="113"/>
+      <c r="LF2" s="113"/>
+      <c r="LG2" s="113"/>
+      <c r="LH2" s="113"/>
+      <c r="LI2" s="113"/>
+      <c r="LJ2" s="113"/>
+      <c r="LK2" s="113"/>
+      <c r="LL2" s="113"/>
+      <c r="LM2" s="113"/>
+      <c r="LN2" s="113"/>
+      <c r="LO2" s="114"/>
+      <c r="LP2" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="LQ2" s="111"/>
-      <c r="LR2" s="111"/>
-      <c r="LS2" s="111"/>
-      <c r="LT2" s="111"/>
-      <c r="LU2" s="111"/>
-      <c r="LV2" s="111"/>
-      <c r="LW2" s="111"/>
-      <c r="LX2" s="111"/>
-      <c r="LY2" s="111"/>
-      <c r="LZ2" s="111"/>
-      <c r="MA2" s="111"/>
-      <c r="MB2" s="111"/>
-      <c r="MC2" s="111"/>
-      <c r="MD2" s="111"/>
-      <c r="ME2" s="111"/>
-      <c r="MF2" s="111"/>
-      <c r="MG2" s="111"/>
-      <c r="MH2" s="111"/>
-      <c r="MI2" s="111"/>
-      <c r="MJ2" s="111"/>
-      <c r="MK2" s="111"/>
-      <c r="ML2" s="111"/>
-      <c r="MM2" s="111"/>
-      <c r="MN2" s="111"/>
-      <c r="MO2" s="111"/>
-      <c r="MP2" s="112"/>
-      <c r="MQ2" s="110" t="s">
+      <c r="LQ2" s="113"/>
+      <c r="LR2" s="113"/>
+      <c r="LS2" s="113"/>
+      <c r="LT2" s="113"/>
+      <c r="LU2" s="113"/>
+      <c r="LV2" s="113"/>
+      <c r="LW2" s="113"/>
+      <c r="LX2" s="113"/>
+      <c r="LY2" s="113"/>
+      <c r="LZ2" s="113"/>
+      <c r="MA2" s="113"/>
+      <c r="MB2" s="113"/>
+      <c r="MC2" s="113"/>
+      <c r="MD2" s="113"/>
+      <c r="ME2" s="113"/>
+      <c r="MF2" s="113"/>
+      <c r="MG2" s="113"/>
+      <c r="MH2" s="113"/>
+      <c r="MI2" s="113"/>
+      <c r="MJ2" s="113"/>
+      <c r="MK2" s="113"/>
+      <c r="ML2" s="113"/>
+      <c r="MM2" s="113"/>
+      <c r="MN2" s="113"/>
+      <c r="MO2" s="113"/>
+      <c r="MP2" s="114"/>
+      <c r="MQ2" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="MR2" s="111"/>
-      <c r="MS2" s="111"/>
-      <c r="MT2" s="111"/>
-      <c r="MU2" s="111"/>
-      <c r="MV2" s="111"/>
-      <c r="MW2" s="111"/>
-      <c r="MX2" s="111"/>
-      <c r="MY2" s="111"/>
-      <c r="MZ2" s="111"/>
-      <c r="NA2" s="111"/>
-      <c r="NB2" s="111"/>
-      <c r="NC2" s="111"/>
-      <c r="ND2" s="111"/>
-      <c r="NE2" s="111"/>
-      <c r="NF2" s="111"/>
-      <c r="NG2" s="111"/>
-      <c r="NH2" s="111"/>
-      <c r="NI2" s="111"/>
-      <c r="NJ2" s="111"/>
-      <c r="NK2" s="111"/>
-      <c r="NL2" s="111"/>
-      <c r="NM2" s="111"/>
-      <c r="NN2" s="111"/>
-      <c r="NO2" s="111"/>
-      <c r="NP2" s="111"/>
-      <c r="NQ2" s="112"/>
-      <c r="NR2" s="110" t="s">
+      <c r="MR2" s="113"/>
+      <c r="MS2" s="113"/>
+      <c r="MT2" s="113"/>
+      <c r="MU2" s="113"/>
+      <c r="MV2" s="113"/>
+      <c r="MW2" s="113"/>
+      <c r="MX2" s="113"/>
+      <c r="MY2" s="113"/>
+      <c r="MZ2" s="113"/>
+      <c r="NA2" s="113"/>
+      <c r="NB2" s="113"/>
+      <c r="NC2" s="113"/>
+      <c r="ND2" s="113"/>
+      <c r="NE2" s="113"/>
+      <c r="NF2" s="113"/>
+      <c r="NG2" s="113"/>
+      <c r="NH2" s="113"/>
+      <c r="NI2" s="113"/>
+      <c r="NJ2" s="113"/>
+      <c r="NK2" s="113"/>
+      <c r="NL2" s="113"/>
+      <c r="NM2" s="113"/>
+      <c r="NN2" s="113"/>
+      <c r="NO2" s="113"/>
+      <c r="NP2" s="113"/>
+      <c r="NQ2" s="114"/>
+      <c r="NR2" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="NS2" s="111"/>
-      <c r="NT2" s="111"/>
-      <c r="NU2" s="111"/>
-      <c r="NV2" s="111"/>
-      <c r="NW2" s="111"/>
-      <c r="NX2" s="111"/>
-      <c r="NY2" s="111"/>
-      <c r="NZ2" s="111"/>
-      <c r="OA2" s="111"/>
-      <c r="OB2" s="111"/>
-      <c r="OC2" s="111"/>
-      <c r="OD2" s="111"/>
-      <c r="OE2" s="111"/>
-      <c r="OF2" s="111"/>
-      <c r="OG2" s="111"/>
-      <c r="OH2" s="111"/>
-      <c r="OI2" s="111"/>
-      <c r="OJ2" s="111"/>
-      <c r="OK2" s="111"/>
-      <c r="OL2" s="111"/>
-      <c r="OM2" s="111"/>
-      <c r="ON2" s="111"/>
-      <c r="OO2" s="111"/>
-      <c r="OP2" s="111"/>
-      <c r="OQ2" s="111"/>
-      <c r="OR2" s="112"/>
-      <c r="OS2" s="110" t="s">
+      <c r="NS2" s="113"/>
+      <c r="NT2" s="113"/>
+      <c r="NU2" s="113"/>
+      <c r="NV2" s="113"/>
+      <c r="NW2" s="113"/>
+      <c r="NX2" s="113"/>
+      <c r="NY2" s="113"/>
+      <c r="NZ2" s="113"/>
+      <c r="OA2" s="113"/>
+      <c r="OB2" s="113"/>
+      <c r="OC2" s="113"/>
+      <c r="OD2" s="113"/>
+      <c r="OE2" s="113"/>
+      <c r="OF2" s="113"/>
+      <c r="OG2" s="113"/>
+      <c r="OH2" s="113"/>
+      <c r="OI2" s="113"/>
+      <c r="OJ2" s="113"/>
+      <c r="OK2" s="113"/>
+      <c r="OL2" s="113"/>
+      <c r="OM2" s="113"/>
+      <c r="ON2" s="113"/>
+      <c r="OO2" s="113"/>
+      <c r="OP2" s="113"/>
+      <c r="OQ2" s="113"/>
+      <c r="OR2" s="114"/>
+      <c r="OS2" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="OT2" s="111"/>
-      <c r="OU2" s="111"/>
-      <c r="OV2" s="111"/>
-      <c r="OW2" s="111"/>
-      <c r="OX2" s="111"/>
-      <c r="OY2" s="111"/>
-      <c r="OZ2" s="111"/>
-      <c r="PA2" s="111"/>
-      <c r="PB2" s="111"/>
-      <c r="PC2" s="111"/>
-      <c r="PD2" s="111"/>
-      <c r="PE2" s="111"/>
-      <c r="PF2" s="111"/>
-      <c r="PG2" s="111"/>
-      <c r="PH2" s="111"/>
-      <c r="PI2" s="111"/>
-      <c r="PJ2" s="111"/>
-      <c r="PK2" s="111"/>
-      <c r="PL2" s="111"/>
-      <c r="PM2" s="111"/>
-      <c r="PN2" s="111"/>
-      <c r="PO2" s="111"/>
-      <c r="PP2" s="111"/>
-      <c r="PQ2" s="111"/>
-      <c r="PR2" s="111"/>
-      <c r="PS2" s="112"/>
+      <c r="OT2" s="113"/>
+      <c r="OU2" s="113"/>
+      <c r="OV2" s="113"/>
+      <c r="OW2" s="113"/>
+      <c r="OX2" s="113"/>
+      <c r="OY2" s="113"/>
+      <c r="OZ2" s="113"/>
+      <c r="PA2" s="113"/>
+      <c r="PB2" s="113"/>
+      <c r="PC2" s="113"/>
+      <c r="PD2" s="113"/>
+      <c r="PE2" s="113"/>
+      <c r="PF2" s="113"/>
+      <c r="PG2" s="113"/>
+      <c r="PH2" s="113"/>
+      <c r="PI2" s="113"/>
+      <c r="PJ2" s="113"/>
+      <c r="PK2" s="113"/>
+      <c r="PL2" s="113"/>
+      <c r="PM2" s="113"/>
+      <c r="PN2" s="113"/>
+      <c r="PO2" s="113"/>
+      <c r="PP2" s="113"/>
+      <c r="PQ2" s="113"/>
+      <c r="PR2" s="113"/>
+      <c r="PS2" s="114"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
@@ -5061,7 +5078,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="114"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5499,7 +5516,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="113" t="str">
+      <c r="B7" s="110" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -5940,7 +5957,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="114"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6378,7 +6395,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="113" t="str">
+      <c r="B9" s="110" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -6819,7 +6836,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="114"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7257,7 +7274,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="113" t="str">
+      <c r="B11" s="110" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7698,7 +7715,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="114"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8136,7 +8153,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="113" t="str">
+      <c r="B13" s="110" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8577,7 +8594,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="114"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -9015,7 +9032,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="113" t="str">
+      <c r="B15" s="110" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9457,7 +9474,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="114"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -9895,7 +9912,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="113" t="str">
+      <c r="B17" s="110" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10336,7 +10353,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="114"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -10774,7 +10791,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="113" t="str">
+      <c r="B19" s="110" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11215,7 +11232,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="114"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11653,7 +11670,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="113" t="str">
+      <c r="B21" s="110" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12094,7 +12111,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="114"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12532,7 +12549,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="113" t="str">
+      <c r="B23" s="110" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -12973,7 +12990,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="114"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13411,7 +13428,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="113" t="str">
+      <c r="B25" s="110" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -13852,7 +13869,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="114"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14290,7 +14307,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="113" t="str">
+      <c r="B27" s="110" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -14731,7 +14748,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="114"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15169,7 +15186,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="113" t="str">
+      <c r="B29" s="110" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15610,7 +15627,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="114"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16048,7 +16065,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="113" t="str">
+      <c r="B31" s="110" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16489,7 +16506,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="114"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -17811,14 +17828,13 @@
   </sheetData>
   <sheetProtection insertRows="0" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="HL2:IL2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="CG2:DG2"/>
-    <mergeCell ref="DH2:EH2"/>
-    <mergeCell ref="EI2:FI2"/>
-    <mergeCell ref="FJ2:GJ2"/>
-    <mergeCell ref="GK2:HK2"/>
+    <mergeCell ref="OS2:PS2"/>
+    <mergeCell ref="IM2:JM2"/>
+    <mergeCell ref="JN2:KN2"/>
+    <mergeCell ref="KO2:LO2"/>
+    <mergeCell ref="LP2:MP2"/>
+    <mergeCell ref="MQ2:NQ2"/>
+    <mergeCell ref="NR2:OR2"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="D2:AD2"/>
@@ -17835,13 +17851,14 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="OS2:PS2"/>
-    <mergeCell ref="IM2:JM2"/>
-    <mergeCell ref="JN2:KN2"/>
-    <mergeCell ref="KO2:LO2"/>
-    <mergeCell ref="LP2:MP2"/>
-    <mergeCell ref="MQ2:NQ2"/>
-    <mergeCell ref="NR2:OR2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="HL2:IL2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="CG2:DG2"/>
+    <mergeCell ref="DH2:EH2"/>
+    <mergeCell ref="EI2:FI2"/>
+    <mergeCell ref="FJ2:GJ2"/>
+    <mergeCell ref="GK2:HK2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C33">
@@ -20512,8 +20529,8 @@
   </sheetPr>
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A55" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A80" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21265,28 +21282,52 @@
       </c>
       <c r="D71" s="13"/>
     </row>
-    <row r="72" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="14"/>
+    <row r="72" spans="1:4" ht="81" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="6">
+        <v>4</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="D72" s="14"/>
     </row>
-    <row r="73" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="14"/>
+    <row r="73" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="6">
+        <v>1</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="D73" s="14"/>
     </row>
-    <row r="74" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="14"/>
+    <row r="74" spans="1:4" ht="243" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="6">
+        <v>20</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="14"/>
+      <c r="A75" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="6">
+        <v>1</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21355,7 +21396,7 @@
       </c>
       <c r="B86" s="76">
         <f>SUM(B71:B85)</f>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C86" s="107" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
MAJ JDT JLZ 09.06.2017
Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Doc/DemoMotJDT-Lopezji.xlsx
+++ b/Doc/DemoMotJDT-Lopezji.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lopezji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Applications\GitRepository\Demomot\Demomot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,10 +33,10 @@
     <definedName name="objPlanifWeek" localSheetId="5">Planning!$A$1:$D$14</definedName>
     <definedName name="objPlanifWeek">PlanificationWeek!$A$1:$D$14</definedName>
     <definedName name="objRealizedWeek" localSheetId="6">achievementWeek!$A$1:$D$19</definedName>
-    <definedName name="objRealizedWeek" localSheetId="7">JNLTRAV!$A$1:$D$7</definedName>
+    <definedName name="objRealizedWeek" localSheetId="7">JNLTRAV!$A$1:$D$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Diagramme!$A$1:$PT$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$277</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$239</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Planning!$A$1:$D$224</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="88">
   <si>
     <t>Module :</t>
   </si>
@@ -309,6 +309,21 @@
   </si>
   <si>
     <t>J'ai chercher comment installer une extension permettant d'écrire du code PHP directement sur typo3. J'ai installé plusieurs extension mais elle ne fonctionnent malheureusement pas avec notre version de typo3. J'ai donc continué à chercher des solutions. J'ai suivi un tutoriel qui montre comment créer un script en php qu'il faudra appeler pour que le code écrit à l'intérieur s'execute mais cela ne fonctionne pas non plus. J'ai continué à chercher des extension et une des extension que j'ai installé a créé une erreur qui rendait l'interface typo3 inutilisable. une erreur apparaissait et ne laissait rien faire. J'ai donc chercher comment désinstaller une extension sans l'interface (donc avec les fichiers) et j'ai trouvé. Il fallait chercher dans le fichier PackageStates.php et mettre en commentaire la dernièrer extension que j'ai installé, ensuite l'interface s'est lancée comme il faut et j'ai désinstallé l'extension. Nous sommes allé chercher Mme hardegger mais nous ne l'avons pas trouvé. En attendant, j'ai continué à faire le background du site en prenant des personnages et en les détourant. Nous avons ensuite trouvé Mme hardegger et elle nous a expliqué qu'il fallait tout simplement créer une extension non pas pour écrire en php mais pour directement effectuer ce que l'on voulait coder en php (donc une extension qui gère les jeux flashs). J'ai regardé un tutoriel et j'ai installé l'extension "extension builder" qui sert à créer des extensions. J'ai vu un peu comment l'extension fonctionne et je vais pouvoir m'y mettre dès la prochaine fois.</t>
+  </si>
+  <si>
+    <t>Daily scrum avec fabien</t>
+  </si>
+  <si>
+    <t>GitKraken est très lent à cause de typo3 (trop volumineux) et nous avons supprimé le gitignore car finalement nous avions besoin de tous les fichier pour bien enregistrer toutes les modification. J'ai aussi du supprimer typo3 qui s'était mis dans ma branche JLZ.</t>
+  </si>
+  <si>
+    <t>J'ai suivi le tutoriel pour savoir comment mettre une authentification sur le site. J'ai du créer un groupe d'utilisateurs admin ainsi que l'utilisateur admin. J'ai implémenté un formulaire de connexion qui apparait quand l'utilisateur n'est pas connecté. Un message apparait aussi lorsqu'aucun utilisateur n'est connecté, il indique qu'il faut se connecter et propose directement à l'utilisateur de le faire avec un formulaire juste en dessous du message. J'ai ensuite brievement expliqué à Fabien afin qu'il puisse implémenter tout ça sur le site. J'ai alors cherché comment publier un jeu en SWF sur une page de façon à ce que l'utilisateur puisse jouer sur le site web mais car je n'y arrivais pas. Quand je voulais "uploader" un jeu, typo3 me disait que le fichier n'était pas compatible. Sur les forums, les adeptes de typo3 disent qu'il faut installer une extension qui permet à typo3 de gérer les fichiers en .swf. Toutes les extension que j'ai pu trouver ne sont pas compatible avec la derniere version de typo3. Soit rien ne se passait, soit une erreur rendait typo3 inutilisable. J'ai donc cherché une alternative à ça et je peux maintenant publier un jeux sur le site mais c'est un peu différent, sur le site est publié un lien de téléchargement pour le jeu. Si le navigateur utilisé est Google Chrome, le jeu s'ouvrira et l'utilisateur joue sur le navigateur et si c'est Firefox ou Internet Explorer, le jeu se télécharge et l'utilisateur n'a qu'à executer le fichier et le jeu se lance. Je cherche maintenant à mettre une image et une description à coté du jeu publié. La description s'affiche comme souhaité mais l'image n'apparait pas. J'ai cherché dans le code de la page et j'ai pu constater que les dimensions de l'image sont 0x0. Aucun moyen de modifier ça quelque part sauf sur le code directement qui permet uniquement de voir à quoi ça pourrait ressembler. Je cherche une solution à mon problème sur internet. Après avoir cherché sur un maximum de sites internet, je n'ai trouvé aucune solution a mon problème, j'ai donc demandé à Mme Hardegger de m'aider et elle m'a donné une piste qui n'a malheureusement pas abouti à une solution. J'ai donc trouvé une alternative. J'ajoute à la page un contenu en HTML et je code en brute la source de l'image afin qu'elle soit visible sur le site. ça fonctionne, J'ai pu mettre en page la structure de l'accueil. Il contient deux jeux (pour le moment) avec une description et une image en guise d'illustration.</t>
+  </si>
+  <si>
+    <t>Mise à jour de GitKraken</t>
+  </si>
+  <si>
+    <t>Mise à jour du journal de travail + correction des dates</t>
   </si>
 </sst>
 </file>
@@ -20527,10 +20542,10 @@
   <sheetPr codeName="Feuil9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I278"/>
+  <dimension ref="A1:I240"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A80" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A61" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20582,248 +20597,255 @@
       </c>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:9" s="81" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="79"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-    </row>
-    <row r="5" spans="1:9" s="81" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+    <row r="4" spans="1:9" s="81" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="76">
-        <f>SUM(B3:B5)</f>
+      <c r="B5" s="76">
+        <f>SUM(B3:B4)</f>
         <v>27</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C5" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="77"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="D5" s="77"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="72">
+      <c r="B7" s="72">
         <v>2</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C7" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D7" s="82">
         <v>42885</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="s">
+    <row r="8" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B8" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C8" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D8" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="9" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B9" s="8">
         <v>15</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="27" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="27" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="37"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="14"/>
+    <row r="13" spans="1:9" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6">
+        <v>5</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="37"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" spans="1:9" ht="40.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="37"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="14"/>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="37"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+    <row r="16" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="76">
+        <f>SUM(B9:B15)</f>
+        <v>27</v>
+      </c>
+      <c r="C16" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="77"/>
       <c r="E16" s="37"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="37"/>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="37"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="76">
-        <f>SUM(B10:B17)</f>
-        <v>27</v>
-      </c>
-      <c r="C18" s="107" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="77"/>
+    <row r="18" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="72">
+        <v>3</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="82">
+        <v>42886</v>
+      </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-    </row>
-    <row r="20" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="72">
+    <row r="19" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="82">
-        <v>42886</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="75" t="s">
+      <c r="B19" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C19" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="74" t="s">
+      <c r="D19" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+    <row r="20" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="6">
+        <v>5</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" ht="216" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="6">
+        <v>13</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>57</v>
       </c>
@@ -20831,317 +20853,358 @@
         <v>5</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:9" ht="216" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="76">
+        <f>SUM(B20:B26)</f>
+        <v>27</v>
+      </c>
+      <c r="C27" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="77"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="78"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+    </row>
+    <row r="29" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="72">
+        <v>4</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="82">
+        <v>42888</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" ht="81" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="6">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B33" s="6">
+        <v>16</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="1:4" ht="54" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="76">
+        <f>SUM(B31:B37)</f>
+        <v>27</v>
+      </c>
+      <c r="C38" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="77"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="78"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="72">
+        <v>5</v>
+      </c>
+      <c r="C40" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="82">
+        <v>42892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:9" ht="27" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="6">
-        <v>5</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="6">
-        <v>2</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="42" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="8">
+        <v>15</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="14"/>
+    </row>
+    <row r="44" spans="1:4" ht="108" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="6">
+        <v>10</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="14"/>
+    </row>
+    <row r="45" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B45" s="6">
         <v>1</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C45" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="76" t="s">
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+    </row>
+    <row r="47" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="76">
-        <f>SUM(B22:B29)</f>
+      <c r="B47" s="76">
+        <f>SUM(B42:B46)</f>
         <v>27</v>
       </c>
-      <c r="C30" s="107" t="s">
+      <c r="C47" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="77"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="78"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-    </row>
-    <row r="32" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="71" t="s">
+      <c r="D47" s="77"/>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="78"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="72">
+      <c r="B49" s="72">
+        <v>6</v>
+      </c>
+      <c r="C49" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="82">
+        <v>42893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="8">
+        <v>1</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" ht="81" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="6">
         <v>4</v>
       </c>
-      <c r="C32" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="82">
-        <v>42888</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="8">
-        <v>1</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" ht="81" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="6">
-        <v>5</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="6">
-        <v>16</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="1:4" ht="54" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="6">
-        <v>3</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="6">
-        <v>1</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="6">
-        <v>1</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-    </row>
-    <row r="42" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-    </row>
-    <row r="43" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-    </row>
-    <row r="44" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="79"/>
-      <c r="B45" s="79"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
-    </row>
-    <row r="46" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="79"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-    </row>
-    <row r="47" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="76">
-        <f>SUM(B34:B47)</f>
-        <v>27</v>
-      </c>
-      <c r="C48" s="107" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="77"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="78"/>
-      <c r="B49" s="78"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-    </row>
-    <row r="50" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="72">
-        <v>5</v>
-      </c>
-      <c r="C50" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="82">
-        <v>42912</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="8">
-        <v>15</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="13"/>
-    </row>
-    <row r="53" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C52" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="14"/>
+    </row>
+    <row r="53" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B53" s="6">
         <v>1</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:4" ht="108" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="243" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B54" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D54" s="14"/>
     </row>
@@ -21153,69 +21216,122 @@
         <v>1</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-    </row>
-    <row r="57" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-    </row>
-    <row r="58" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-    </row>
-    <row r="59" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-    </row>
-    <row r="60" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
+    <row r="56" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+    </row>
+    <row r="57" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="76">
+        <f>SUM(B51:B56)</f>
+        <v>27</v>
+      </c>
+      <c r="C57" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="77"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="78"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="78"/>
+    </row>
+    <row r="59" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="72">
+        <v>7</v>
+      </c>
+      <c r="C59" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="82">
+        <v>42895</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="74" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-    </row>
-    <row r="62" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="14"/>
+      <c r="A61" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="8">
+        <v>1</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="13"/>
+    </row>
+    <row r="62" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="6">
+        <v>2</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="D62" s="14"/>
     </row>
-    <row r="63" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="14"/>
+    <row r="63" spans="1:4" ht="378" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="6">
+        <v>21</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="79"/>
-      <c r="B64" s="79"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
+      <c r="A64" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="6">
+        <v>2</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="79"/>
-      <c r="B65" s="79"/>
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
+      <c r="A65" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="6">
+        <v>1</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
@@ -21228,7 +21344,7 @@
         <v>22</v>
       </c>
       <c r="B67" s="76">
-        <f>SUM(B52:B66)</f>
+        <f>SUM(B61:B66)</f>
         <v>27</v>
       </c>
       <c r="C67" s="107" t="s">
@@ -21247,13 +21363,13 @@
         <v>14</v>
       </c>
       <c r="B69" s="72">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C69" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="82">
-        <v>42919</v>
+        <v>42933</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21271,63 +21387,33 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" s="8">
-        <v>1</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>66</v>
-      </c>
+      <c r="A71" s="9"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="13"/>
     </row>
-    <row r="72" spans="1:4" ht="81" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B72" s="6">
-        <v>4</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>78</v>
-      </c>
+    <row r="72" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="14"/>
       <c r="D72" s="14"/>
     </row>
-    <row r="73" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="6">
-        <v>1</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>80</v>
-      </c>
+    <row r="73" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="14"/>
     </row>
-    <row r="74" spans="1:4" ht="243" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="6">
-        <v>20</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>82</v>
-      </c>
+    <row r="74" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B75" s="6">
-        <v>1</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="A75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21396,7 +21482,7 @@
       </c>
       <c r="B86" s="76">
         <f>SUM(B71:B85)</f>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C86" s="107" t="s">
         <v>44</v>
@@ -21414,13 +21500,13 @@
         <v>14</v>
       </c>
       <c r="B88" s="72">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C88" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D88" s="82">
-        <v>42926</v>
+        <v>42940</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21551,13 +21637,13 @@
         <v>14</v>
       </c>
       <c r="B107" s="72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C107" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D107" s="82">
-        <v>42933</v>
+        <v>42947</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21688,13 +21774,13 @@
         <v>14</v>
       </c>
       <c r="B126" s="72">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C126" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D126" s="82">
-        <v>42940</v>
+        <v>42954</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21825,13 +21911,13 @@
         <v>14</v>
       </c>
       <c r="B145" s="72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C145" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D145" s="82">
-        <v>42947</v>
+        <v>42961</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21962,13 +22048,13 @@
         <v>14</v>
       </c>
       <c r="B164" s="72">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C164" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D164" s="82">
-        <v>42954</v>
+        <v>42968</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -22099,13 +22185,13 @@
         <v>14</v>
       </c>
       <c r="B183" s="72">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C183" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D183" s="82">
-        <v>42961</v>
+        <v>42975</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -22236,13 +22322,13 @@
         <v>14</v>
       </c>
       <c r="B202" s="72">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C202" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D202" s="82">
-        <v>42968</v>
+        <v>42982</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -22373,13 +22459,13 @@
         <v>14</v>
       </c>
       <c r="B221" s="72">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C221" s="73" t="s">
         <v>23</v>
       </c>
       <c r="D221" s="82">
-        <v>42975</v>
+        <v>42989</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -22499,301 +22585,27 @@
       </c>
       <c r="D238" s="77"/>
     </row>
-    <row r="239" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A239" s="78"/>
       <c r="B239" s="78"/>
       <c r="C239" s="78"/>
       <c r="D239" s="78"/>
     </row>
-    <row r="240" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B240" s="72">
-        <v>15</v>
-      </c>
-      <c r="C240" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D240" s="82">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B241" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C241" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D241" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A242" s="9"/>
-      <c r="B242" s="8"/>
-      <c r="C242" s="13"/>
-      <c r="D242" s="13"/>
-    </row>
-    <row r="243" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A243" s="5"/>
-      <c r="B243" s="6"/>
-      <c r="C243" s="14"/>
-      <c r="D243" s="14"/>
-    </row>
-    <row r="244" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A244" s="5"/>
-      <c r="B244" s="6"/>
-      <c r="C244" s="14"/>
-      <c r="D244" s="14"/>
-    </row>
-    <row r="245" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A245" s="5"/>
-      <c r="B245" s="6"/>
-      <c r="C245" s="14"/>
-      <c r="D245" s="14"/>
-    </row>
-    <row r="246" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A246" s="5"/>
-      <c r="B246" s="6"/>
-      <c r="C246" s="14"/>
-      <c r="D246" s="14"/>
-    </row>
-    <row r="247" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A247" s="5"/>
-      <c r="B247" s="6"/>
-      <c r="C247" s="14"/>
-      <c r="D247" s="14"/>
-    </row>
-    <row r="248" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A248" s="5"/>
-      <c r="B248" s="6"/>
-      <c r="C248" s="14"/>
-      <c r="D248" s="14"/>
-    </row>
-    <row r="249" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A249" s="5"/>
-      <c r="B249" s="6"/>
-      <c r="C249" s="14"/>
-      <c r="D249" s="14"/>
-    </row>
-    <row r="250" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A250" s="5"/>
-      <c r="B250" s="6"/>
-      <c r="C250" s="14"/>
-      <c r="D250" s="14"/>
-    </row>
-    <row r="251" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A251" s="6"/>
-      <c r="B251" s="6"/>
-      <c r="C251" s="14"/>
-      <c r="D251" s="14"/>
-    </row>
-    <row r="252" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A252" s="6"/>
-      <c r="B252" s="6"/>
-      <c r="C252" s="14"/>
-      <c r="D252" s="14"/>
-    </row>
-    <row r="253" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A253" s="6"/>
-      <c r="B253" s="6"/>
-      <c r="C253" s="14"/>
-      <c r="D253" s="14"/>
-    </row>
-    <row r="254" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A254" s="79"/>
-      <c r="B254" s="79"/>
-      <c r="C254" s="80"/>
-      <c r="D254" s="80"/>
-    </row>
-    <row r="255" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A255" s="79"/>
-      <c r="B255" s="79"/>
-      <c r="C255" s="80"/>
-      <c r="D255" s="80"/>
-    </row>
-    <row r="256" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="7"/>
-      <c r="B256" s="7"/>
-      <c r="C256" s="15"/>
-      <c r="D256" s="15"/>
-    </row>
-    <row r="257" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B257" s="76">
-        <f>SUM(B242:B256)</f>
-        <v>0</v>
-      </c>
-      <c r="C257" s="107" t="s">
-        <v>44</v>
-      </c>
-      <c r="D257" s="77"/>
-    </row>
-    <row r="258" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="78"/>
-      <c r="B258" s="78"/>
-      <c r="C258" s="78"/>
-      <c r="D258" s="78"/>
-    </row>
-    <row r="259" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B259" s="72">
-        <v>16</v>
-      </c>
-      <c r="C259" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D259" s="82">
-        <v>42989</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B260" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C260" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D260" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A261" s="9"/>
-      <c r="B261" s="8"/>
-      <c r="C261" s="13"/>
-      <c r="D261" s="13"/>
-    </row>
-    <row r="262" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A262" s="5"/>
-      <c r="B262" s="6"/>
-      <c r="C262" s="14"/>
-      <c r="D262" s="14"/>
-    </row>
-    <row r="263" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A263" s="5"/>
-      <c r="B263" s="6"/>
-      <c r="C263" s="14"/>
-      <c r="D263" s="14"/>
-    </row>
-    <row r="264" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A264" s="5"/>
-      <c r="B264" s="6"/>
-      <c r="C264" s="14"/>
-      <c r="D264" s="14"/>
-    </row>
-    <row r="265" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A265" s="5"/>
-      <c r="B265" s="6"/>
-      <c r="C265" s="14"/>
-      <c r="D265" s="14"/>
-    </row>
-    <row r="266" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A266" s="5"/>
-      <c r="B266" s="6"/>
-      <c r="C266" s="14"/>
-      <c r="D266" s="14"/>
-    </row>
-    <row r="267" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A267" s="5"/>
-      <c r="B267" s="6"/>
-      <c r="C267" s="14"/>
-      <c r="D267" s="14"/>
-    </row>
-    <row r="268" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A268" s="5"/>
-      <c r="B268" s="6"/>
-      <c r="C268" s="14"/>
-      <c r="D268" s="14"/>
-    </row>
-    <row r="269" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A269" s="5"/>
-      <c r="B269" s="6"/>
-      <c r="C269" s="14"/>
-      <c r="D269" s="14"/>
-    </row>
-    <row r="270" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A270" s="6"/>
-      <c r="B270" s="6"/>
-      <c r="C270" s="14"/>
-      <c r="D270" s="14"/>
-    </row>
-    <row r="271" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A271" s="6"/>
-      <c r="B271" s="6"/>
-      <c r="C271" s="14"/>
-      <c r="D271" s="14"/>
-    </row>
-    <row r="272" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A272" s="6"/>
-      <c r="B272" s="6"/>
-      <c r="C272" s="14"/>
-      <c r="D272" s="14"/>
-    </row>
-    <row r="273" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A273" s="79"/>
-      <c r="B273" s="79"/>
-      <c r="C273" s="80"/>
-      <c r="D273" s="80"/>
-    </row>
-    <row r="274" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A274" s="79"/>
-      <c r="B274" s="79"/>
-      <c r="C274" s="80"/>
-      <c r="D274" s="80"/>
-    </row>
-    <row r="275" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="7"/>
-      <c r="B275" s="7"/>
-      <c r="C275" s="15"/>
-      <c r="D275" s="15"/>
-    </row>
-    <row r="276" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B276" s="76">
-        <f>SUM(B261:B275)</f>
-        <v>0</v>
-      </c>
-      <c r="C276" s="107" t="s">
-        <v>44</v>
-      </c>
-      <c r="D276" s="77"/>
-    </row>
-    <row r="277" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A277" s="78"/>
-      <c r="B277" s="78"/>
-      <c r="C277" s="78"/>
-      <c r="D277" s="78"/>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A278" s="106" t="s">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="106" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F15:F16 B52:B66 B71:B85 B90:B104 B109:B123 B128:B142 B147:B161 B166:B180 B185:B199 B204:B218 B223:B237 B242:B256 B261:B275 B3:B5 B22:B29 B10:B17 B34:B47">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F14 B71:B85 B90:B104 B109:B123 B128:B142 B147:B161 B166:B180 B185:B199 B204:B218 B223:B237 B61:B66 B51:B56 B42:B46 B31:B37 B20:B26 B9:B15 B3:B4">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B6 B18 B30 B48 B67 B86 B105 B124 B143 B162 B181 B200 B219 B238 B257 B276">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B5 B16 B27 B38 B47 B57 B67 B86 B105 B124 B143 B162 B181 B200 B219 B238">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A52:A66 A71:A85 A90:A104 A109:A123 A128:A142 A147:A161 A166:A180 A185:A199 A204:A218 A223:A237 A242:A256 A261:A275 A3:A5 A22:A29 A10:A17 A34:A47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A85 A90:A104 A109:A123 A128:A142 A147:A161 A166:A180 A185:A199 A204:A218 A223:A237 A61:A66 A51:A56 A42:A46 A31:A37 A20:A26 A9:A15 A3:A4">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
MAJ JDT JLZ 13.06.2017
Mise à jour
</commit_message>
<xml_diff>
--- a/Doc/DemoMotJDT-Lopezji.xlsx
+++ b/Doc/DemoMotJDT-Lopezji.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Applications\GitRepository\Demomot\Demomot\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lopezji\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
     <definedName name="objRealizedWeek" localSheetId="7">JNLTRAV!$A$1:$D$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Diagramme!$A$1:$PT$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$239</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$241</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Planning!$A$1:$D$224</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="96">
   <si>
     <t>Module :</t>
   </si>
@@ -324,6 +324,30 @@
   </si>
   <si>
     <t>Mise à jour du journal de travail + correction des dates</t>
+  </si>
+  <si>
+    <t>Mise à jour gitkraken de nos données (relativement lent à cause du nombre de fichiers)</t>
+  </si>
+  <si>
+    <t>séance de classe</t>
+  </si>
+  <si>
+    <t>Pause de midi en + (les Lundis)</t>
+  </si>
+  <si>
+    <t>Background bientôt terminé</t>
+  </si>
+  <si>
+    <t>Daily Scrum seul (Fabien Pittier passe ses examens)</t>
+  </si>
+  <si>
+    <t>J'a installé la bonne version de l'extension "extension builder" qui permet de créer des extensions. J'ai fait un peu de découverte sur cette extension (avec Fabien Pittier) J'ai essayé de créer une extension mais finalement Fabien le faisait sur son pc aussi alors j'ai décidé de regarder avec lui afin de comprendre ensemble. C'est assez compliqué et difficile de comprendre son utilisation. Nous sommes aussi descendu pour voir Mme Hardegger afin d'avoir une très courte introduction sur l'extension. Même avec son expliquation le sujet reste assez vague.</t>
+  </si>
+  <si>
+    <t>Je regarde encore des tutos pour créer des extensions vu que c'est la seule chose qu'il nous manque sur laquelle on peut continuer. J'essaye de reproduire les actions décrites dans le tutoriel. C'est assez vague et je ne comprends pas toujours à quoi sert certaines options utilisées. J'ai créé une extension et je la vois dans la liste d'extensions. Le tuto ne dit pas ce qu'il faut faire en suite avec ça et je ne vois pas trop quoi faire. J'essaye de trouver comment employer l'extension créée.</t>
+  </si>
+  <si>
+    <t>Design du site terminé. Tout le côté droit est rempli de personnages différents de jeux différents. Le côté gauche n'est une symétrie horizontale. (Si le temps le permet, le côté gauche sera aussi d'autres personnages différents)</t>
   </si>
 </sst>
 </file>
@@ -1413,12 +1437,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1427,6 +1445,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3198,27 +3222,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3248,27 +3272,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3306,470 +3330,470 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="114"/>
-      <c r="AE2" s="112" t="s">
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="113"/>
-      <c r="AI2" s="113"/>
-      <c r="AJ2" s="113"/>
-      <c r="AK2" s="113"/>
-      <c r="AL2" s="113"/>
-      <c r="AM2" s="113"/>
-      <c r="AN2" s="113"/>
-      <c r="AO2" s="113"/>
-      <c r="AP2" s="113"/>
-      <c r="AQ2" s="113"/>
-      <c r="AR2" s="113"/>
-      <c r="AS2" s="113"/>
-      <c r="AT2" s="113"/>
-      <c r="AU2" s="113"/>
-      <c r="AV2" s="113"/>
-      <c r="AW2" s="113"/>
-      <c r="AX2" s="113"/>
-      <c r="AY2" s="113"/>
-      <c r="AZ2" s="113"/>
-      <c r="BA2" s="113"/>
-      <c r="BB2" s="113"/>
-      <c r="BC2" s="113"/>
-      <c r="BD2" s="113"/>
-      <c r="BE2" s="114"/>
-      <c r="BF2" s="112" t="s">
+      <c r="AF2" s="111"/>
+      <c r="AG2" s="111"/>
+      <c r="AH2" s="111"/>
+      <c r="AI2" s="111"/>
+      <c r="AJ2" s="111"/>
+      <c r="AK2" s="111"/>
+      <c r="AL2" s="111"/>
+      <c r="AM2" s="111"/>
+      <c r="AN2" s="111"/>
+      <c r="AO2" s="111"/>
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="111"/>
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="111"/>
+      <c r="AU2" s="111"/>
+      <c r="AV2" s="111"/>
+      <c r="AW2" s="111"/>
+      <c r="AX2" s="111"/>
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="111"/>
+      <c r="BA2" s="111"/>
+      <c r="BB2" s="111"/>
+      <c r="BC2" s="111"/>
+      <c r="BD2" s="111"/>
+      <c r="BE2" s="112"/>
+      <c r="BF2" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="BG2" s="113"/>
-      <c r="BH2" s="113"/>
-      <c r="BI2" s="113"/>
-      <c r="BJ2" s="113"/>
-      <c r="BK2" s="113"/>
-      <c r="BL2" s="113"/>
-      <c r="BM2" s="113"/>
-      <c r="BN2" s="113"/>
-      <c r="BO2" s="113"/>
-      <c r="BP2" s="113"/>
-      <c r="BQ2" s="113"/>
-      <c r="BR2" s="113"/>
-      <c r="BS2" s="113"/>
-      <c r="BT2" s="113"/>
-      <c r="BU2" s="113"/>
-      <c r="BV2" s="113"/>
-      <c r="BW2" s="113"/>
-      <c r="BX2" s="113"/>
-      <c r="BY2" s="113"/>
-      <c r="BZ2" s="113"/>
-      <c r="CA2" s="113"/>
-      <c r="CB2" s="113"/>
-      <c r="CC2" s="113"/>
-      <c r="CD2" s="113"/>
-      <c r="CE2" s="113"/>
-      <c r="CF2" s="114"/>
-      <c r="CG2" s="112" t="s">
+      <c r="BG2" s="111"/>
+      <c r="BH2" s="111"/>
+      <c r="BI2" s="111"/>
+      <c r="BJ2" s="111"/>
+      <c r="BK2" s="111"/>
+      <c r="BL2" s="111"/>
+      <c r="BM2" s="111"/>
+      <c r="BN2" s="111"/>
+      <c r="BO2" s="111"/>
+      <c r="BP2" s="111"/>
+      <c r="BQ2" s="111"/>
+      <c r="BR2" s="111"/>
+      <c r="BS2" s="111"/>
+      <c r="BT2" s="111"/>
+      <c r="BU2" s="111"/>
+      <c r="BV2" s="111"/>
+      <c r="BW2" s="111"/>
+      <c r="BX2" s="111"/>
+      <c r="BY2" s="111"/>
+      <c r="BZ2" s="111"/>
+      <c r="CA2" s="111"/>
+      <c r="CB2" s="111"/>
+      <c r="CC2" s="111"/>
+      <c r="CD2" s="111"/>
+      <c r="CE2" s="111"/>
+      <c r="CF2" s="112"/>
+      <c r="CG2" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="CH2" s="113"/>
-      <c r="CI2" s="113"/>
-      <c r="CJ2" s="113"/>
-      <c r="CK2" s="113"/>
-      <c r="CL2" s="113"/>
-      <c r="CM2" s="113"/>
-      <c r="CN2" s="113"/>
-      <c r="CO2" s="113"/>
-      <c r="CP2" s="113"/>
-      <c r="CQ2" s="113"/>
-      <c r="CR2" s="113"/>
-      <c r="CS2" s="113"/>
-      <c r="CT2" s="113"/>
-      <c r="CU2" s="113"/>
-      <c r="CV2" s="113"/>
-      <c r="CW2" s="113"/>
-      <c r="CX2" s="113"/>
-      <c r="CY2" s="113"/>
-      <c r="CZ2" s="113"/>
-      <c r="DA2" s="113"/>
-      <c r="DB2" s="113"/>
-      <c r="DC2" s="113"/>
-      <c r="DD2" s="113"/>
-      <c r="DE2" s="113"/>
-      <c r="DF2" s="113"/>
-      <c r="DG2" s="114"/>
-      <c r="DH2" s="112" t="s">
+      <c r="CH2" s="111"/>
+      <c r="CI2" s="111"/>
+      <c r="CJ2" s="111"/>
+      <c r="CK2" s="111"/>
+      <c r="CL2" s="111"/>
+      <c r="CM2" s="111"/>
+      <c r="CN2" s="111"/>
+      <c r="CO2" s="111"/>
+      <c r="CP2" s="111"/>
+      <c r="CQ2" s="111"/>
+      <c r="CR2" s="111"/>
+      <c r="CS2" s="111"/>
+      <c r="CT2" s="111"/>
+      <c r="CU2" s="111"/>
+      <c r="CV2" s="111"/>
+      <c r="CW2" s="111"/>
+      <c r="CX2" s="111"/>
+      <c r="CY2" s="111"/>
+      <c r="CZ2" s="111"/>
+      <c r="DA2" s="111"/>
+      <c r="DB2" s="111"/>
+      <c r="DC2" s="111"/>
+      <c r="DD2" s="111"/>
+      <c r="DE2" s="111"/>
+      <c r="DF2" s="111"/>
+      <c r="DG2" s="112"/>
+      <c r="DH2" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="DI2" s="113"/>
-      <c r="DJ2" s="113"/>
-      <c r="DK2" s="113"/>
-      <c r="DL2" s="113"/>
-      <c r="DM2" s="113"/>
-      <c r="DN2" s="113"/>
-      <c r="DO2" s="113"/>
-      <c r="DP2" s="113"/>
-      <c r="DQ2" s="113"/>
-      <c r="DR2" s="113"/>
-      <c r="DS2" s="113"/>
-      <c r="DT2" s="113"/>
-      <c r="DU2" s="113"/>
-      <c r="DV2" s="113"/>
-      <c r="DW2" s="113"/>
-      <c r="DX2" s="113"/>
-      <c r="DY2" s="113"/>
-      <c r="DZ2" s="113"/>
-      <c r="EA2" s="113"/>
-      <c r="EB2" s="113"/>
-      <c r="EC2" s="113"/>
-      <c r="ED2" s="113"/>
-      <c r="EE2" s="113"/>
-      <c r="EF2" s="113"/>
-      <c r="EG2" s="113"/>
-      <c r="EH2" s="114"/>
-      <c r="EI2" s="112" t="s">
+      <c r="DI2" s="111"/>
+      <c r="DJ2" s="111"/>
+      <c r="DK2" s="111"/>
+      <c r="DL2" s="111"/>
+      <c r="DM2" s="111"/>
+      <c r="DN2" s="111"/>
+      <c r="DO2" s="111"/>
+      <c r="DP2" s="111"/>
+      <c r="DQ2" s="111"/>
+      <c r="DR2" s="111"/>
+      <c r="DS2" s="111"/>
+      <c r="DT2" s="111"/>
+      <c r="DU2" s="111"/>
+      <c r="DV2" s="111"/>
+      <c r="DW2" s="111"/>
+      <c r="DX2" s="111"/>
+      <c r="DY2" s="111"/>
+      <c r="DZ2" s="111"/>
+      <c r="EA2" s="111"/>
+      <c r="EB2" s="111"/>
+      <c r="EC2" s="111"/>
+      <c r="ED2" s="111"/>
+      <c r="EE2" s="111"/>
+      <c r="EF2" s="111"/>
+      <c r="EG2" s="111"/>
+      <c r="EH2" s="112"/>
+      <c r="EI2" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="113"/>
-      <c r="EK2" s="113"/>
-      <c r="EL2" s="113"/>
-      <c r="EM2" s="113"/>
-      <c r="EN2" s="113"/>
-      <c r="EO2" s="113"/>
-      <c r="EP2" s="113"/>
-      <c r="EQ2" s="113"/>
-      <c r="ER2" s="113"/>
-      <c r="ES2" s="113"/>
-      <c r="ET2" s="113"/>
-      <c r="EU2" s="113"/>
-      <c r="EV2" s="113"/>
-      <c r="EW2" s="113"/>
-      <c r="EX2" s="113"/>
-      <c r="EY2" s="113"/>
-      <c r="EZ2" s="113"/>
-      <c r="FA2" s="113"/>
-      <c r="FB2" s="113"/>
-      <c r="FC2" s="113"/>
-      <c r="FD2" s="113"/>
-      <c r="FE2" s="113"/>
-      <c r="FF2" s="113"/>
-      <c r="FG2" s="113"/>
-      <c r="FH2" s="113"/>
-      <c r="FI2" s="114"/>
-      <c r="FJ2" s="112" t="s">
+      <c r="EJ2" s="111"/>
+      <c r="EK2" s="111"/>
+      <c r="EL2" s="111"/>
+      <c r="EM2" s="111"/>
+      <c r="EN2" s="111"/>
+      <c r="EO2" s="111"/>
+      <c r="EP2" s="111"/>
+      <c r="EQ2" s="111"/>
+      <c r="ER2" s="111"/>
+      <c r="ES2" s="111"/>
+      <c r="ET2" s="111"/>
+      <c r="EU2" s="111"/>
+      <c r="EV2" s="111"/>
+      <c r="EW2" s="111"/>
+      <c r="EX2" s="111"/>
+      <c r="EY2" s="111"/>
+      <c r="EZ2" s="111"/>
+      <c r="FA2" s="111"/>
+      <c r="FB2" s="111"/>
+      <c r="FC2" s="111"/>
+      <c r="FD2" s="111"/>
+      <c r="FE2" s="111"/>
+      <c r="FF2" s="111"/>
+      <c r="FG2" s="111"/>
+      <c r="FH2" s="111"/>
+      <c r="FI2" s="112"/>
+      <c r="FJ2" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="FK2" s="113"/>
-      <c r="FL2" s="113"/>
-      <c r="FM2" s="113"/>
-      <c r="FN2" s="113"/>
-      <c r="FO2" s="113"/>
-      <c r="FP2" s="113"/>
-      <c r="FQ2" s="113"/>
-      <c r="FR2" s="113"/>
-      <c r="FS2" s="113"/>
-      <c r="FT2" s="113"/>
-      <c r="FU2" s="113"/>
-      <c r="FV2" s="113"/>
-      <c r="FW2" s="113"/>
-      <c r="FX2" s="113"/>
-      <c r="FY2" s="113"/>
-      <c r="FZ2" s="113"/>
-      <c r="GA2" s="113"/>
-      <c r="GB2" s="113"/>
-      <c r="GC2" s="113"/>
-      <c r="GD2" s="113"/>
-      <c r="GE2" s="113"/>
-      <c r="GF2" s="113"/>
-      <c r="GG2" s="113"/>
-      <c r="GH2" s="113"/>
-      <c r="GI2" s="113"/>
-      <c r="GJ2" s="114"/>
-      <c r="GK2" s="112" t="s">
+      <c r="FK2" s="111"/>
+      <c r="FL2" s="111"/>
+      <c r="FM2" s="111"/>
+      <c r="FN2" s="111"/>
+      <c r="FO2" s="111"/>
+      <c r="FP2" s="111"/>
+      <c r="FQ2" s="111"/>
+      <c r="FR2" s="111"/>
+      <c r="FS2" s="111"/>
+      <c r="FT2" s="111"/>
+      <c r="FU2" s="111"/>
+      <c r="FV2" s="111"/>
+      <c r="FW2" s="111"/>
+      <c r="FX2" s="111"/>
+      <c r="FY2" s="111"/>
+      <c r="FZ2" s="111"/>
+      <c r="GA2" s="111"/>
+      <c r="GB2" s="111"/>
+      <c r="GC2" s="111"/>
+      <c r="GD2" s="111"/>
+      <c r="GE2" s="111"/>
+      <c r="GF2" s="111"/>
+      <c r="GG2" s="111"/>
+      <c r="GH2" s="111"/>
+      <c r="GI2" s="111"/>
+      <c r="GJ2" s="112"/>
+      <c r="GK2" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="GL2" s="113"/>
-      <c r="GM2" s="113"/>
-      <c r="GN2" s="113"/>
-      <c r="GO2" s="113"/>
-      <c r="GP2" s="113"/>
-      <c r="GQ2" s="113"/>
-      <c r="GR2" s="113"/>
-      <c r="GS2" s="113"/>
-      <c r="GT2" s="113"/>
-      <c r="GU2" s="113"/>
-      <c r="GV2" s="113"/>
-      <c r="GW2" s="113"/>
-      <c r="GX2" s="113"/>
-      <c r="GY2" s="113"/>
-      <c r="GZ2" s="113"/>
-      <c r="HA2" s="113"/>
-      <c r="HB2" s="113"/>
-      <c r="HC2" s="113"/>
-      <c r="HD2" s="113"/>
-      <c r="HE2" s="113"/>
-      <c r="HF2" s="113"/>
-      <c r="HG2" s="113"/>
-      <c r="HH2" s="113"/>
-      <c r="HI2" s="113"/>
-      <c r="HJ2" s="113"/>
-      <c r="HK2" s="114"/>
-      <c r="HL2" s="112" t="s">
+      <c r="GL2" s="111"/>
+      <c r="GM2" s="111"/>
+      <c r="GN2" s="111"/>
+      <c r="GO2" s="111"/>
+      <c r="GP2" s="111"/>
+      <c r="GQ2" s="111"/>
+      <c r="GR2" s="111"/>
+      <c r="GS2" s="111"/>
+      <c r="GT2" s="111"/>
+      <c r="GU2" s="111"/>
+      <c r="GV2" s="111"/>
+      <c r="GW2" s="111"/>
+      <c r="GX2" s="111"/>
+      <c r="GY2" s="111"/>
+      <c r="GZ2" s="111"/>
+      <c r="HA2" s="111"/>
+      <c r="HB2" s="111"/>
+      <c r="HC2" s="111"/>
+      <c r="HD2" s="111"/>
+      <c r="HE2" s="111"/>
+      <c r="HF2" s="111"/>
+      <c r="HG2" s="111"/>
+      <c r="HH2" s="111"/>
+      <c r="HI2" s="111"/>
+      <c r="HJ2" s="111"/>
+      <c r="HK2" s="112"/>
+      <c r="HL2" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="HM2" s="113"/>
-      <c r="HN2" s="113"/>
-      <c r="HO2" s="113"/>
-      <c r="HP2" s="113"/>
-      <c r="HQ2" s="113"/>
-      <c r="HR2" s="113"/>
-      <c r="HS2" s="113"/>
-      <c r="HT2" s="113"/>
-      <c r="HU2" s="113"/>
-      <c r="HV2" s="113"/>
-      <c r="HW2" s="113"/>
-      <c r="HX2" s="113"/>
-      <c r="HY2" s="113"/>
-      <c r="HZ2" s="113"/>
-      <c r="IA2" s="113"/>
-      <c r="IB2" s="113"/>
-      <c r="IC2" s="113"/>
-      <c r="ID2" s="113"/>
-      <c r="IE2" s="113"/>
-      <c r="IF2" s="113"/>
-      <c r="IG2" s="113"/>
-      <c r="IH2" s="113"/>
-      <c r="II2" s="113"/>
-      <c r="IJ2" s="113"/>
-      <c r="IK2" s="113"/>
-      <c r="IL2" s="114"/>
-      <c r="IM2" s="112" t="s">
+      <c r="HM2" s="111"/>
+      <c r="HN2" s="111"/>
+      <c r="HO2" s="111"/>
+      <c r="HP2" s="111"/>
+      <c r="HQ2" s="111"/>
+      <c r="HR2" s="111"/>
+      <c r="HS2" s="111"/>
+      <c r="HT2" s="111"/>
+      <c r="HU2" s="111"/>
+      <c r="HV2" s="111"/>
+      <c r="HW2" s="111"/>
+      <c r="HX2" s="111"/>
+      <c r="HY2" s="111"/>
+      <c r="HZ2" s="111"/>
+      <c r="IA2" s="111"/>
+      <c r="IB2" s="111"/>
+      <c r="IC2" s="111"/>
+      <c r="ID2" s="111"/>
+      <c r="IE2" s="111"/>
+      <c r="IF2" s="111"/>
+      <c r="IG2" s="111"/>
+      <c r="IH2" s="111"/>
+      <c r="II2" s="111"/>
+      <c r="IJ2" s="111"/>
+      <c r="IK2" s="111"/>
+      <c r="IL2" s="112"/>
+      <c r="IM2" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="IN2" s="113"/>
-      <c r="IO2" s="113"/>
-      <c r="IP2" s="113"/>
-      <c r="IQ2" s="113"/>
-      <c r="IR2" s="113"/>
-      <c r="IS2" s="113"/>
-      <c r="IT2" s="113"/>
-      <c r="IU2" s="113"/>
-      <c r="IV2" s="113"/>
-      <c r="IW2" s="113"/>
-      <c r="IX2" s="113"/>
-      <c r="IY2" s="113"/>
-      <c r="IZ2" s="113"/>
-      <c r="JA2" s="113"/>
-      <c r="JB2" s="113"/>
-      <c r="JC2" s="113"/>
-      <c r="JD2" s="113"/>
-      <c r="JE2" s="113"/>
-      <c r="JF2" s="113"/>
-      <c r="JG2" s="113"/>
-      <c r="JH2" s="113"/>
-      <c r="JI2" s="113"/>
-      <c r="JJ2" s="113"/>
-      <c r="JK2" s="113"/>
-      <c r="JL2" s="113"/>
-      <c r="JM2" s="114"/>
-      <c r="JN2" s="112" t="s">
+      <c r="IN2" s="111"/>
+      <c r="IO2" s="111"/>
+      <c r="IP2" s="111"/>
+      <c r="IQ2" s="111"/>
+      <c r="IR2" s="111"/>
+      <c r="IS2" s="111"/>
+      <c r="IT2" s="111"/>
+      <c r="IU2" s="111"/>
+      <c r="IV2" s="111"/>
+      <c r="IW2" s="111"/>
+      <c r="IX2" s="111"/>
+      <c r="IY2" s="111"/>
+      <c r="IZ2" s="111"/>
+      <c r="JA2" s="111"/>
+      <c r="JB2" s="111"/>
+      <c r="JC2" s="111"/>
+      <c r="JD2" s="111"/>
+      <c r="JE2" s="111"/>
+      <c r="JF2" s="111"/>
+      <c r="JG2" s="111"/>
+      <c r="JH2" s="111"/>
+      <c r="JI2" s="111"/>
+      <c r="JJ2" s="111"/>
+      <c r="JK2" s="111"/>
+      <c r="JL2" s="111"/>
+      <c r="JM2" s="112"/>
+      <c r="JN2" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="JO2" s="113"/>
-      <c r="JP2" s="113"/>
-      <c r="JQ2" s="113"/>
-      <c r="JR2" s="113"/>
-      <c r="JS2" s="113"/>
-      <c r="JT2" s="113"/>
-      <c r="JU2" s="113"/>
-      <c r="JV2" s="113"/>
-      <c r="JW2" s="113"/>
-      <c r="JX2" s="113"/>
-      <c r="JY2" s="113"/>
-      <c r="JZ2" s="113"/>
-      <c r="KA2" s="113"/>
-      <c r="KB2" s="113"/>
-      <c r="KC2" s="113"/>
-      <c r="KD2" s="113"/>
-      <c r="KE2" s="113"/>
-      <c r="KF2" s="113"/>
-      <c r="KG2" s="113"/>
-      <c r="KH2" s="113"/>
-      <c r="KI2" s="113"/>
-      <c r="KJ2" s="113"/>
-      <c r="KK2" s="113"/>
-      <c r="KL2" s="113"/>
-      <c r="KM2" s="113"/>
-      <c r="KN2" s="114"/>
-      <c r="KO2" s="112" t="s">
+      <c r="JO2" s="111"/>
+      <c r="JP2" s="111"/>
+      <c r="JQ2" s="111"/>
+      <c r="JR2" s="111"/>
+      <c r="JS2" s="111"/>
+      <c r="JT2" s="111"/>
+      <c r="JU2" s="111"/>
+      <c r="JV2" s="111"/>
+      <c r="JW2" s="111"/>
+      <c r="JX2" s="111"/>
+      <c r="JY2" s="111"/>
+      <c r="JZ2" s="111"/>
+      <c r="KA2" s="111"/>
+      <c r="KB2" s="111"/>
+      <c r="KC2" s="111"/>
+      <c r="KD2" s="111"/>
+      <c r="KE2" s="111"/>
+      <c r="KF2" s="111"/>
+      <c r="KG2" s="111"/>
+      <c r="KH2" s="111"/>
+      <c r="KI2" s="111"/>
+      <c r="KJ2" s="111"/>
+      <c r="KK2" s="111"/>
+      <c r="KL2" s="111"/>
+      <c r="KM2" s="111"/>
+      <c r="KN2" s="112"/>
+      <c r="KO2" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="KP2" s="113"/>
-      <c r="KQ2" s="113"/>
-      <c r="KR2" s="113"/>
-      <c r="KS2" s="113"/>
-      <c r="KT2" s="113"/>
-      <c r="KU2" s="113"/>
-      <c r="KV2" s="113"/>
-      <c r="KW2" s="113"/>
-      <c r="KX2" s="113"/>
-      <c r="KY2" s="113"/>
-      <c r="KZ2" s="113"/>
-      <c r="LA2" s="113"/>
-      <c r="LB2" s="113"/>
-      <c r="LC2" s="113"/>
-      <c r="LD2" s="113"/>
-      <c r="LE2" s="113"/>
-      <c r="LF2" s="113"/>
-      <c r="LG2" s="113"/>
-      <c r="LH2" s="113"/>
-      <c r="LI2" s="113"/>
-      <c r="LJ2" s="113"/>
-      <c r="LK2" s="113"/>
-      <c r="LL2" s="113"/>
-      <c r="LM2" s="113"/>
-      <c r="LN2" s="113"/>
-      <c r="LO2" s="114"/>
-      <c r="LP2" s="112" t="s">
+      <c r="KP2" s="111"/>
+      <c r="KQ2" s="111"/>
+      <c r="KR2" s="111"/>
+      <c r="KS2" s="111"/>
+      <c r="KT2" s="111"/>
+      <c r="KU2" s="111"/>
+      <c r="KV2" s="111"/>
+      <c r="KW2" s="111"/>
+      <c r="KX2" s="111"/>
+      <c r="KY2" s="111"/>
+      <c r="KZ2" s="111"/>
+      <c r="LA2" s="111"/>
+      <c r="LB2" s="111"/>
+      <c r="LC2" s="111"/>
+      <c r="LD2" s="111"/>
+      <c r="LE2" s="111"/>
+      <c r="LF2" s="111"/>
+      <c r="LG2" s="111"/>
+      <c r="LH2" s="111"/>
+      <c r="LI2" s="111"/>
+      <c r="LJ2" s="111"/>
+      <c r="LK2" s="111"/>
+      <c r="LL2" s="111"/>
+      <c r="LM2" s="111"/>
+      <c r="LN2" s="111"/>
+      <c r="LO2" s="112"/>
+      <c r="LP2" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="LQ2" s="113"/>
-      <c r="LR2" s="113"/>
-      <c r="LS2" s="113"/>
-      <c r="LT2" s="113"/>
-      <c r="LU2" s="113"/>
-      <c r="LV2" s="113"/>
-      <c r="LW2" s="113"/>
-      <c r="LX2" s="113"/>
-      <c r="LY2" s="113"/>
-      <c r="LZ2" s="113"/>
-      <c r="MA2" s="113"/>
-      <c r="MB2" s="113"/>
-      <c r="MC2" s="113"/>
-      <c r="MD2" s="113"/>
-      <c r="ME2" s="113"/>
-      <c r="MF2" s="113"/>
-      <c r="MG2" s="113"/>
-      <c r="MH2" s="113"/>
-      <c r="MI2" s="113"/>
-      <c r="MJ2" s="113"/>
-      <c r="MK2" s="113"/>
-      <c r="ML2" s="113"/>
-      <c r="MM2" s="113"/>
-      <c r="MN2" s="113"/>
-      <c r="MO2" s="113"/>
-      <c r="MP2" s="114"/>
-      <c r="MQ2" s="112" t="s">
+      <c r="LQ2" s="111"/>
+      <c r="LR2" s="111"/>
+      <c r="LS2" s="111"/>
+      <c r="LT2" s="111"/>
+      <c r="LU2" s="111"/>
+      <c r="LV2" s="111"/>
+      <c r="LW2" s="111"/>
+      <c r="LX2" s="111"/>
+      <c r="LY2" s="111"/>
+      <c r="LZ2" s="111"/>
+      <c r="MA2" s="111"/>
+      <c r="MB2" s="111"/>
+      <c r="MC2" s="111"/>
+      <c r="MD2" s="111"/>
+      <c r="ME2" s="111"/>
+      <c r="MF2" s="111"/>
+      <c r="MG2" s="111"/>
+      <c r="MH2" s="111"/>
+      <c r="MI2" s="111"/>
+      <c r="MJ2" s="111"/>
+      <c r="MK2" s="111"/>
+      <c r="ML2" s="111"/>
+      <c r="MM2" s="111"/>
+      <c r="MN2" s="111"/>
+      <c r="MO2" s="111"/>
+      <c r="MP2" s="112"/>
+      <c r="MQ2" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="MR2" s="113"/>
-      <c r="MS2" s="113"/>
-      <c r="MT2" s="113"/>
-      <c r="MU2" s="113"/>
-      <c r="MV2" s="113"/>
-      <c r="MW2" s="113"/>
-      <c r="MX2" s="113"/>
-      <c r="MY2" s="113"/>
-      <c r="MZ2" s="113"/>
-      <c r="NA2" s="113"/>
-      <c r="NB2" s="113"/>
-      <c r="NC2" s="113"/>
-      <c r="ND2" s="113"/>
-      <c r="NE2" s="113"/>
-      <c r="NF2" s="113"/>
-      <c r="NG2" s="113"/>
-      <c r="NH2" s="113"/>
-      <c r="NI2" s="113"/>
-      <c r="NJ2" s="113"/>
-      <c r="NK2" s="113"/>
-      <c r="NL2" s="113"/>
-      <c r="NM2" s="113"/>
-      <c r="NN2" s="113"/>
-      <c r="NO2" s="113"/>
-      <c r="NP2" s="113"/>
-      <c r="NQ2" s="114"/>
-      <c r="NR2" s="112" t="s">
+      <c r="MR2" s="111"/>
+      <c r="MS2" s="111"/>
+      <c r="MT2" s="111"/>
+      <c r="MU2" s="111"/>
+      <c r="MV2" s="111"/>
+      <c r="MW2" s="111"/>
+      <c r="MX2" s="111"/>
+      <c r="MY2" s="111"/>
+      <c r="MZ2" s="111"/>
+      <c r="NA2" s="111"/>
+      <c r="NB2" s="111"/>
+      <c r="NC2" s="111"/>
+      <c r="ND2" s="111"/>
+      <c r="NE2" s="111"/>
+      <c r="NF2" s="111"/>
+      <c r="NG2" s="111"/>
+      <c r="NH2" s="111"/>
+      <c r="NI2" s="111"/>
+      <c r="NJ2" s="111"/>
+      <c r="NK2" s="111"/>
+      <c r="NL2" s="111"/>
+      <c r="NM2" s="111"/>
+      <c r="NN2" s="111"/>
+      <c r="NO2" s="111"/>
+      <c r="NP2" s="111"/>
+      <c r="NQ2" s="112"/>
+      <c r="NR2" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="NS2" s="113"/>
-      <c r="NT2" s="113"/>
-      <c r="NU2" s="113"/>
-      <c r="NV2" s="113"/>
-      <c r="NW2" s="113"/>
-      <c r="NX2" s="113"/>
-      <c r="NY2" s="113"/>
-      <c r="NZ2" s="113"/>
-      <c r="OA2" s="113"/>
-      <c r="OB2" s="113"/>
-      <c r="OC2" s="113"/>
-      <c r="OD2" s="113"/>
-      <c r="OE2" s="113"/>
-      <c r="OF2" s="113"/>
-      <c r="OG2" s="113"/>
-      <c r="OH2" s="113"/>
-      <c r="OI2" s="113"/>
-      <c r="OJ2" s="113"/>
-      <c r="OK2" s="113"/>
-      <c r="OL2" s="113"/>
-      <c r="OM2" s="113"/>
-      <c r="ON2" s="113"/>
-      <c r="OO2" s="113"/>
-      <c r="OP2" s="113"/>
-      <c r="OQ2" s="113"/>
-      <c r="OR2" s="114"/>
-      <c r="OS2" s="112" t="s">
+      <c r="NS2" s="111"/>
+      <c r="NT2" s="111"/>
+      <c r="NU2" s="111"/>
+      <c r="NV2" s="111"/>
+      <c r="NW2" s="111"/>
+      <c r="NX2" s="111"/>
+      <c r="NY2" s="111"/>
+      <c r="NZ2" s="111"/>
+      <c r="OA2" s="111"/>
+      <c r="OB2" s="111"/>
+      <c r="OC2" s="111"/>
+      <c r="OD2" s="111"/>
+      <c r="OE2" s="111"/>
+      <c r="OF2" s="111"/>
+      <c r="OG2" s="111"/>
+      <c r="OH2" s="111"/>
+      <c r="OI2" s="111"/>
+      <c r="OJ2" s="111"/>
+      <c r="OK2" s="111"/>
+      <c r="OL2" s="111"/>
+      <c r="OM2" s="111"/>
+      <c r="ON2" s="111"/>
+      <c r="OO2" s="111"/>
+      <c r="OP2" s="111"/>
+      <c r="OQ2" s="111"/>
+      <c r="OR2" s="112"/>
+      <c r="OS2" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="OT2" s="113"/>
-      <c r="OU2" s="113"/>
-      <c r="OV2" s="113"/>
-      <c r="OW2" s="113"/>
-      <c r="OX2" s="113"/>
-      <c r="OY2" s="113"/>
-      <c r="OZ2" s="113"/>
-      <c r="PA2" s="113"/>
-      <c r="PB2" s="113"/>
-      <c r="PC2" s="113"/>
-      <c r="PD2" s="113"/>
-      <c r="PE2" s="113"/>
-      <c r="PF2" s="113"/>
-      <c r="PG2" s="113"/>
-      <c r="PH2" s="113"/>
-      <c r="PI2" s="113"/>
-      <c r="PJ2" s="113"/>
-      <c r="PK2" s="113"/>
-      <c r="PL2" s="113"/>
-      <c r="PM2" s="113"/>
-      <c r="PN2" s="113"/>
-      <c r="PO2" s="113"/>
-      <c r="PP2" s="113"/>
-      <c r="PQ2" s="113"/>
-      <c r="PR2" s="113"/>
-      <c r="PS2" s="114"/>
+      <c r="OT2" s="111"/>
+      <c r="OU2" s="111"/>
+      <c r="OV2" s="111"/>
+      <c r="OW2" s="111"/>
+      <c r="OX2" s="111"/>
+      <c r="OY2" s="111"/>
+      <c r="OZ2" s="111"/>
+      <c r="PA2" s="111"/>
+      <c r="PB2" s="111"/>
+      <c r="PC2" s="111"/>
+      <c r="PD2" s="111"/>
+      <c r="PE2" s="111"/>
+      <c r="PF2" s="111"/>
+      <c r="PG2" s="111"/>
+      <c r="PH2" s="111"/>
+      <c r="PI2" s="111"/>
+      <c r="PJ2" s="111"/>
+      <c r="PK2" s="111"/>
+      <c r="PL2" s="111"/>
+      <c r="PM2" s="111"/>
+      <c r="PN2" s="111"/>
+      <c r="PO2" s="111"/>
+      <c r="PP2" s="111"/>
+      <c r="PQ2" s="111"/>
+      <c r="PR2" s="111"/>
+      <c r="PS2" s="112"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
@@ -5093,7 +5117,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="111"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5531,7 +5555,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="110" t="str">
+      <c r="B7" s="113" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -5972,7 +5996,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="111"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6410,7 +6434,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="110" t="str">
+      <c r="B9" s="113" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -6851,7 +6875,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="111"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7289,7 +7313,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="110" t="str">
+      <c r="B11" s="113" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7730,7 +7754,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="111"/>
+      <c r="B12" s="114"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8168,7 +8192,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="110" t="str">
+      <c r="B13" s="113" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8609,7 +8633,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="111"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -9047,7 +9071,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="110" t="str">
+      <c r="B15" s="113" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9489,7 +9513,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="111"/>
+      <c r="B16" s="114"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -9927,7 +9951,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="110" t="str">
+      <c r="B17" s="113" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10368,7 +10392,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="111"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -10806,7 +10830,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="110" t="str">
+      <c r="B19" s="113" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11247,7 +11271,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="111"/>
+      <c r="B20" s="114"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11685,7 +11709,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="110" t="str">
+      <c r="B21" s="113" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12126,7 +12150,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="111"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12564,7 +12588,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="110" t="str">
+      <c r="B23" s="113" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -13005,7 +13029,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="111"/>
+      <c r="B24" s="114"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13443,7 +13467,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="110" t="str">
+      <c r="B25" s="113" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -13884,7 +13908,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="111"/>
+      <c r="B26" s="114"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14322,7 +14346,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="110" t="str">
+      <c r="B27" s="113" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -14763,7 +14787,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="111"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15201,7 +15225,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="110" t="str">
+      <c r="B29" s="113" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15642,7 +15666,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="111"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16080,7 +16104,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="110" t="str">
+      <c r="B31" s="113" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16521,7 +16545,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="111"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -17843,13 +17867,14 @@
   </sheetData>
   <sheetProtection insertRows="0" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="OS2:PS2"/>
-    <mergeCell ref="IM2:JM2"/>
-    <mergeCell ref="JN2:KN2"/>
-    <mergeCell ref="KO2:LO2"/>
-    <mergeCell ref="LP2:MP2"/>
-    <mergeCell ref="MQ2:NQ2"/>
-    <mergeCell ref="NR2:OR2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="HL2:IL2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="CG2:DG2"/>
+    <mergeCell ref="DH2:EH2"/>
+    <mergeCell ref="EI2:FI2"/>
+    <mergeCell ref="FJ2:GJ2"/>
+    <mergeCell ref="GK2:HK2"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="D2:AD2"/>
@@ -17866,14 +17891,13 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="HL2:IL2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="CG2:DG2"/>
-    <mergeCell ref="DH2:EH2"/>
-    <mergeCell ref="EI2:FI2"/>
-    <mergeCell ref="FJ2:GJ2"/>
-    <mergeCell ref="GK2:HK2"/>
+    <mergeCell ref="OS2:PS2"/>
+    <mergeCell ref="IM2:JM2"/>
+    <mergeCell ref="JN2:KN2"/>
+    <mergeCell ref="KO2:LO2"/>
+    <mergeCell ref="LP2:MP2"/>
+    <mergeCell ref="MQ2:NQ2"/>
+    <mergeCell ref="NR2:OR2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C33">
@@ -20542,10 +20566,10 @@
   <sheetPr codeName="Feuil9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I240"/>
+  <dimension ref="A1:I242"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A61" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A88" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20590,7 +20614,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="8">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>65</v>
@@ -20598,9 +20622,15 @@
       <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:9" s="81" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -21369,7 +21399,7 @@
         <v>23</v>
       </c>
       <c r="D69" s="82">
-        <v>42933</v>
+        <v>42898</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21387,45 +21417,87 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A71" s="9"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="13"/>
+      <c r="A71" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="8">
+        <v>1</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="D71" s="13"/>
     </row>
     <row r="72" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="14"/>
+      <c r="A72" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="6">
+        <v>2</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="D72" s="14"/>
     </row>
-    <row r="73" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="14"/>
+    <row r="73" spans="1:4" ht="94.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" s="6">
+        <v>7</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="D73" s="14"/>
     </row>
     <row r="74" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="14"/>
+      <c r="A74" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="6">
+        <v>3</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>90</v>
+      </c>
       <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="14"/>
+      <c r="A75" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="6">
+        <v>2</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="5"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="14"/>
+      <c r="A76" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="6">
+        <v>11</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="D76" s="14"/>
     </row>
     <row r="77" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="14"/>
+      <c r="A77" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21441,13 +21513,13 @@
       <c r="D79" s="14"/>
     </row>
     <row r="80" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="6"/>
+      <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
     </row>
     <row r="81" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="6"/>
+      <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
@@ -21459,116 +21531,152 @@
       <c r="D82" s="14"/>
     </row>
     <row r="83" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A83" s="79"/>
-      <c r="B83" s="79"/>
-      <c r="C83" s="80"/>
-      <c r="D83" s="80"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
     </row>
     <row r="84" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="79"/>
-      <c r="B84" s="79"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="80"/>
-    </row>
-    <row r="85" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="76" t="s">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+    </row>
+    <row r="85" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A85" s="79"/>
+      <c r="B85" s="79"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="80"/>
+    </row>
+    <row r="86" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A86" s="79"/>
+      <c r="B86" s="79"/>
+      <c r="C86" s="80"/>
+      <c r="D86" s="80"/>
+    </row>
+    <row r="87" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+    </row>
+    <row r="88" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B86" s="76">
-        <f>SUM(B71:B85)</f>
-        <v>0</v>
-      </c>
-      <c r="C86" s="107" t="s">
+      <c r="B88" s="76">
+        <f>SUM(B71:B87)</f>
+        <v>27</v>
+      </c>
+      <c r="C88" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D86" s="77"/>
-    </row>
-    <row r="87" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="78"/>
-      <c r="B87" s="78"/>
-      <c r="C87" s="78"/>
-      <c r="D87" s="78"/>
-    </row>
-    <row r="88" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="71" t="s">
+      <c r="D88" s="77"/>
+    </row>
+    <row r="89" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="78"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="78"/>
+      <c r="D89" s="78"/>
+    </row>
+    <row r="90" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="72">
+      <c r="B90" s="72">
         <v>9</v>
       </c>
-      <c r="C88" s="73" t="s">
+      <c r="C90" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D88" s="82">
-        <v>42940</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="74" t="s">
+      <c r="D90" s="82">
+        <v>42899</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="75" t="s">
+      <c r="B91" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="74" t="s">
+      <c r="C91" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D89" s="74" t="s">
+      <c r="D91" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="9"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-    </row>
-    <row r="91" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-    </row>
     <row r="92" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="5"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
+      <c r="A92" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" s="8">
+        <v>15</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" s="13"/>
     </row>
     <row r="93" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="14"/>
+      <c r="A93" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93" s="6">
+        <v>1</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="D93" s="14"/>
     </row>
-    <row r="94" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="5"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="14"/>
+    <row r="94" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B94" s="6">
+        <v>5</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="D94" s="14"/>
     </row>
-    <row r="95" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="5"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="14"/>
+    <row r="95" spans="1:4" ht="81" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B95" s="6">
+        <v>4</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="D95" s="14"/>
     </row>
     <row r="96" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="5"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="14"/>
+      <c r="A96" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B96" s="6">
+        <v>1</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="5"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="14"/>
+      <c r="A97" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="6">
+        <v>1</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D97" s="14"/>
     </row>
     <row r="98" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21578,13 +21686,13 @@
       <c r="D98" s="14"/>
     </row>
     <row r="99" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
+      <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="C99" s="14"/>
       <c r="D99" s="14"/>
     </row>
     <row r="100" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A100" s="6"/>
+      <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="14"/>
       <c r="D100" s="14"/>
@@ -21596,87 +21704,87 @@
       <c r="D101" s="14"/>
     </row>
     <row r="102" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A102" s="79"/>
-      <c r="B102" s="79"/>
-      <c r="C102" s="80"/>
-      <c r="D102" s="80"/>
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
     </row>
     <row r="103" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="79"/>
-      <c r="B103" s="79"/>
-      <c r="C103" s="80"/>
-      <c r="D103" s="80"/>
-    </row>
-    <row r="104" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-    </row>
-    <row r="105" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="76" t="s">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+    </row>
+    <row r="104" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A104" s="79"/>
+      <c r="B104" s="79"/>
+      <c r="C104" s="80"/>
+      <c r="D104" s="80"/>
+    </row>
+    <row r="105" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A105" s="79"/>
+      <c r="B105" s="79"/>
+      <c r="C105" s="80"/>
+      <c r="D105" s="80"/>
+    </row>
+    <row r="106" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
+    </row>
+    <row r="107" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="76">
-        <f>SUM(B90:B104)</f>
-        <v>0</v>
-      </c>
-      <c r="C105" s="107" t="s">
+      <c r="B107" s="76">
+        <f>SUM(B92:B106)</f>
+        <v>27</v>
+      </c>
+      <c r="C107" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D105" s="77"/>
-    </row>
-    <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="78"/>
-      <c r="B106" s="78"/>
-      <c r="C106" s="78"/>
-      <c r="D106" s="78"/>
-    </row>
-    <row r="107" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="71" t="s">
+      <c r="D107" s="77"/>
+    </row>
+    <row r="108" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="78"/>
+      <c r="B108" s="78"/>
+      <c r="C108" s="78"/>
+      <c r="D108" s="78"/>
+    </row>
+    <row r="109" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B107" s="72">
+      <c r="B109" s="72">
         <v>10</v>
       </c>
-      <c r="C107" s="73" t="s">
+      <c r="C109" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D107" s="82">
+      <c r="D109" s="82">
         <v>42947</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="74" t="s">
+    <row r="110" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B108" s="75" t="s">
+      <c r="B110" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C108" s="74" t="s">
+      <c r="C110" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D108" s="74" t="s">
+      <c r="D110" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A109" s="9"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="13"/>
-    </row>
-    <row r="110" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A110" s="5"/>
-      <c r="B110" s="6"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-    </row>
     <row r="111" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A111" s="5"/>
-      <c r="B111" s="6"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
+      <c r="A111" s="9"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
     </row>
     <row r="112" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
@@ -21715,13 +21823,13 @@
       <c r="D117" s="14"/>
     </row>
     <row r="118" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A118" s="6"/>
+      <c r="A118" s="5"/>
       <c r="B118" s="6"/>
       <c r="C118" s="14"/>
       <c r="D118" s="14"/>
     </row>
     <row r="119" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A119" s="6"/>
+      <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="C119" s="14"/>
       <c r="D119" s="14"/>
@@ -21733,87 +21841,87 @@
       <c r="D120" s="14"/>
     </row>
     <row r="121" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A121" s="79"/>
-      <c r="B121" s="79"/>
-      <c r="C121" s="80"/>
-      <c r="D121" s="80"/>
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
     </row>
     <row r="122" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A122" s="79"/>
-      <c r="B122" s="79"/>
-      <c r="C122" s="80"/>
-      <c r="D122" s="80"/>
-    </row>
-    <row r="123" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15"/>
-    </row>
-    <row r="124" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="76" t="s">
+      <c r="A122" s="6"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+    </row>
+    <row r="123" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="79"/>
+      <c r="B123" s="79"/>
+      <c r="C123" s="80"/>
+      <c r="D123" s="80"/>
+    </row>
+    <row r="124" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A124" s="79"/>
+      <c r="B124" s="79"/>
+      <c r="C124" s="80"/>
+      <c r="D124" s="80"/>
+    </row>
+    <row r="125" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+    </row>
+    <row r="126" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B124" s="76">
-        <f>SUM(B109:B123)</f>
+      <c r="B126" s="76">
+        <f>SUM(B111:B125)</f>
         <v>0</v>
       </c>
-      <c r="C124" s="107" t="s">
+      <c r="C126" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D124" s="77"/>
-    </row>
-    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="78"/>
-      <c r="B125" s="78"/>
-      <c r="C125" s="78"/>
-      <c r="D125" s="78"/>
-    </row>
-    <row r="126" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="71" t="s">
+      <c r="D126" s="77"/>
+    </row>
+    <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="78"/>
+      <c r="B127" s="78"/>
+      <c r="C127" s="78"/>
+      <c r="D127" s="78"/>
+    </row>
+    <row r="128" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B126" s="72">
+      <c r="B128" s="72">
         <v>11</v>
       </c>
-      <c r="C126" s="73" t="s">
+      <c r="C128" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D126" s="82">
+      <c r="D128" s="82">
         <v>42954</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="74" t="s">
+    <row r="129" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B127" s="75" t="s">
+      <c r="B129" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C127" s="74" t="s">
+      <c r="C129" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D127" s="74" t="s">
+      <c r="D129" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A128" s="9"/>
-      <c r="B128" s="8"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-    </row>
-    <row r="129" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="5"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-    </row>
     <row r="130" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A130" s="5"/>
-      <c r="B130" s="6"/>
-      <c r="C130" s="14"/>
-      <c r="D130" s="14"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
     </row>
     <row r="131" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
@@ -21852,13 +21960,13 @@
       <c r="D136" s="14"/>
     </row>
     <row r="137" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A137" s="6"/>
+      <c r="A137" s="5"/>
       <c r="B137" s="6"/>
       <c r="C137" s="14"/>
       <c r="D137" s="14"/>
     </row>
     <row r="138" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A138" s="6"/>
+      <c r="A138" s="5"/>
       <c r="B138" s="6"/>
       <c r="C138" s="14"/>
       <c r="D138" s="14"/>
@@ -21870,87 +21978,87 @@
       <c r="D139" s="14"/>
     </row>
     <row r="140" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A140" s="79"/>
-      <c r="B140" s="79"/>
-      <c r="C140" s="80"/>
-      <c r="D140" s="80"/>
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
     </row>
     <row r="141" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A141" s="79"/>
-      <c r="B141" s="79"/>
-      <c r="C141" s="80"/>
-      <c r="D141" s="80"/>
-    </row>
-    <row r="142" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-    </row>
-    <row r="143" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="76" t="s">
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14"/>
+    </row>
+    <row r="142" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A142" s="79"/>
+      <c r="B142" s="79"/>
+      <c r="C142" s="80"/>
+      <c r="D142" s="80"/>
+    </row>
+    <row r="143" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A143" s="79"/>
+      <c r="B143" s="79"/>
+      <c r="C143" s="80"/>
+      <c r="D143" s="80"/>
+    </row>
+    <row r="144" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="15"/>
+      <c r="D144" s="15"/>
+    </row>
+    <row r="145" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B143" s="76">
-        <f>SUM(B128:B142)</f>
+      <c r="B145" s="76">
+        <f>SUM(B130:B144)</f>
         <v>0</v>
       </c>
-      <c r="C143" s="107" t="s">
+      <c r="C145" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D143" s="77"/>
-    </row>
-    <row r="144" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="78"/>
-      <c r="B144" s="78"/>
-      <c r="C144" s="78"/>
-      <c r="D144" s="78"/>
-    </row>
-    <row r="145" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="71" t="s">
+      <c r="D145" s="77"/>
+    </row>
+    <row r="146" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="78"/>
+      <c r="B146" s="78"/>
+      <c r="C146" s="78"/>
+      <c r="D146" s="78"/>
+    </row>
+    <row r="147" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B145" s="72">
+      <c r="B147" s="72">
         <v>12</v>
       </c>
-      <c r="C145" s="73" t="s">
+      <c r="C147" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D145" s="82">
+      <c r="D147" s="82">
         <v>42961</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="74" t="s">
+    <row r="148" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B146" s="75" t="s">
+      <c r="B148" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C146" s="74" t="s">
+      <c r="C148" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D146" s="74" t="s">
+      <c r="D148" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A147" s="9"/>
-      <c r="B147" s="8"/>
-      <c r="C147" s="13"/>
-      <c r="D147" s="13"/>
-    </row>
-    <row r="148" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A148" s="5"/>
-      <c r="B148" s="6"/>
-      <c r="C148" s="14"/>
-      <c r="D148" s="14"/>
-    </row>
     <row r="149" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A149" s="5"/>
-      <c r="B149" s="6"/>
-      <c r="C149" s="14"/>
-      <c r="D149" s="14"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
     </row>
     <row r="150" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A150" s="5"/>
@@ -21989,13 +22097,13 @@
       <c r="D155" s="14"/>
     </row>
     <row r="156" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A156" s="6"/>
+      <c r="A156" s="5"/>
       <c r="B156" s="6"/>
       <c r="C156" s="14"/>
       <c r="D156" s="14"/>
     </row>
     <row r="157" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A157" s="6"/>
+      <c r="A157" s="5"/>
       <c r="B157" s="6"/>
       <c r="C157" s="14"/>
       <c r="D157" s="14"/>
@@ -22007,87 +22115,87 @@
       <c r="D158" s="14"/>
     </row>
     <row r="159" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A159" s="79"/>
-      <c r="B159" s="79"/>
-      <c r="C159" s="80"/>
-      <c r="D159" s="80"/>
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
     </row>
     <row r="160" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A160" s="79"/>
-      <c r="B160" s="79"/>
-      <c r="C160" s="80"/>
-      <c r="D160" s="80"/>
-    </row>
-    <row r="161" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="15"/>
-      <c r="D161" s="15"/>
-    </row>
-    <row r="162" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="76" t="s">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="14"/>
+      <c r="D160" s="14"/>
+    </row>
+    <row r="161" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A161" s="79"/>
+      <c r="B161" s="79"/>
+      <c r="C161" s="80"/>
+      <c r="D161" s="80"/>
+    </row>
+    <row r="162" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A162" s="79"/>
+      <c r="B162" s="79"/>
+      <c r="C162" s="80"/>
+      <c r="D162" s="80"/>
+    </row>
+    <row r="163" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="7"/>
+      <c r="B163" s="7"/>
+      <c r="C163" s="15"/>
+      <c r="D163" s="15"/>
+    </row>
+    <row r="164" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B162" s="76">
-        <f>SUM(B147:B161)</f>
+      <c r="B164" s="76">
+        <f>SUM(B149:B163)</f>
         <v>0</v>
       </c>
-      <c r="C162" s="107" t="s">
+      <c r="C164" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D162" s="77"/>
-    </row>
-    <row r="163" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="78"/>
-      <c r="B163" s="78"/>
-      <c r="C163" s="78"/>
-      <c r="D163" s="78"/>
-    </row>
-    <row r="164" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="71" t="s">
+      <c r="D164" s="77"/>
+    </row>
+    <row r="165" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="78"/>
+      <c r="B165" s="78"/>
+      <c r="C165" s="78"/>
+      <c r="D165" s="78"/>
+    </row>
+    <row r="166" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="72">
+      <c r="B166" s="72">
         <v>13</v>
       </c>
-      <c r="C164" s="73" t="s">
+      <c r="C166" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D164" s="82">
+      <c r="D166" s="82">
         <v>42968</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="74" t="s">
+    <row r="167" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B165" s="75" t="s">
+      <c r="B167" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C165" s="74" t="s">
+      <c r="C167" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D165" s="74" t="s">
+      <c r="D167" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A166" s="9"/>
-      <c r="B166" s="8"/>
-      <c r="C166" s="13"/>
-      <c r="D166" s="13"/>
-    </row>
-    <row r="167" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A167" s="5"/>
-      <c r="B167" s="6"/>
-      <c r="C167" s="14"/>
-      <c r="D167" s="14"/>
-    </row>
     <row r="168" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="5"/>
-      <c r="B168" s="6"/>
-      <c r="C168" s="14"/>
-      <c r="D168" s="14"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
     </row>
     <row r="169" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A169" s="5"/>
@@ -22126,13 +22234,13 @@
       <c r="D174" s="14"/>
     </row>
     <row r="175" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A175" s="6"/>
+      <c r="A175" s="5"/>
       <c r="B175" s="6"/>
       <c r="C175" s="14"/>
       <c r="D175" s="14"/>
     </row>
     <row r="176" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A176" s="6"/>
+      <c r="A176" s="5"/>
       <c r="B176" s="6"/>
       <c r="C176" s="14"/>
       <c r="D176" s="14"/>
@@ -22144,87 +22252,87 @@
       <c r="D177" s="14"/>
     </row>
     <row r="178" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A178" s="79"/>
-      <c r="B178" s="79"/>
-      <c r="C178" s="80"/>
-      <c r="D178" s="80"/>
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="14"/>
     </row>
     <row r="179" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A179" s="79"/>
-      <c r="B179" s="79"/>
-      <c r="C179" s="80"/>
-      <c r="D179" s="80"/>
-    </row>
-    <row r="180" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="7"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-    </row>
-    <row r="181" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="76" t="s">
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="14"/>
+      <c r="D179" s="14"/>
+    </row>
+    <row r="180" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A180" s="79"/>
+      <c r="B180" s="79"/>
+      <c r="C180" s="80"/>
+      <c r="D180" s="80"/>
+    </row>
+    <row r="181" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A181" s="79"/>
+      <c r="B181" s="79"/>
+      <c r="C181" s="80"/>
+      <c r="D181" s="80"/>
+    </row>
+    <row r="182" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="15"/>
+      <c r="D182" s="15"/>
+    </row>
+    <row r="183" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B181" s="76">
-        <f>SUM(B166:B180)</f>
+      <c r="B183" s="76">
+        <f>SUM(B168:B182)</f>
         <v>0</v>
       </c>
-      <c r="C181" s="107" t="s">
+      <c r="C183" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D181" s="77"/>
-    </row>
-    <row r="182" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="78"/>
-      <c r="B182" s="78"/>
-      <c r="C182" s="78"/>
-      <c r="D182" s="78"/>
-    </row>
-    <row r="183" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="71" t="s">
+      <c r="D183" s="77"/>
+    </row>
+    <row r="184" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="78"/>
+      <c r="B184" s="78"/>
+      <c r="C184" s="78"/>
+      <c r="D184" s="78"/>
+    </row>
+    <row r="185" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B183" s="72">
+      <c r="B185" s="72">
         <v>14</v>
       </c>
-      <c r="C183" s="73" t="s">
+      <c r="C185" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D183" s="82">
+      <c r="D185" s="82">
         <v>42975</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="74" t="s">
+    <row r="186" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B184" s="75" t="s">
+      <c r="B186" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C184" s="74" t="s">
+      <c r="C186" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D184" s="74" t="s">
+      <c r="D186" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A185" s="9"/>
-      <c r="B185" s="8"/>
-      <c r="C185" s="13"/>
-      <c r="D185" s="13"/>
-    </row>
-    <row r="186" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A186" s="5"/>
-      <c r="B186" s="6"/>
-      <c r="C186" s="14"/>
-      <c r="D186" s="14"/>
-    </row>
     <row r="187" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A187" s="5"/>
-      <c r="B187" s="6"/>
-      <c r="C187" s="14"/>
-      <c r="D187" s="14"/>
+      <c r="A187" s="9"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="13"/>
+      <c r="D187" s="13"/>
     </row>
     <row r="188" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A188" s="5"/>
@@ -22263,13 +22371,13 @@
       <c r="D193" s="14"/>
     </row>
     <row r="194" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A194" s="6"/>
+      <c r="A194" s="5"/>
       <c r="B194" s="6"/>
       <c r="C194" s="14"/>
       <c r="D194" s="14"/>
     </row>
     <row r="195" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A195" s="6"/>
+      <c r="A195" s="5"/>
       <c r="B195" s="6"/>
       <c r="C195" s="14"/>
       <c r="D195" s="14"/>
@@ -22281,87 +22389,87 @@
       <c r="D196" s="14"/>
     </row>
     <row r="197" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A197" s="79"/>
-      <c r="B197" s="79"/>
-      <c r="C197" s="80"/>
-      <c r="D197" s="80"/>
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="14"/>
+      <c r="D197" s="14"/>
     </row>
     <row r="198" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A198" s="79"/>
-      <c r="B198" s="79"/>
-      <c r="C198" s="80"/>
-      <c r="D198" s="80"/>
-    </row>
-    <row r="199" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="7"/>
-      <c r="B199" s="7"/>
-      <c r="C199" s="15"/>
-      <c r="D199" s="15"/>
-    </row>
-    <row r="200" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="76" t="s">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="14"/>
+      <c r="D198" s="14"/>
+    </row>
+    <row r="199" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A199" s="79"/>
+      <c r="B199" s="79"/>
+      <c r="C199" s="80"/>
+      <c r="D199" s="80"/>
+    </row>
+    <row r="200" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A200" s="79"/>
+      <c r="B200" s="79"/>
+      <c r="C200" s="80"/>
+      <c r="D200" s="80"/>
+    </row>
+    <row r="201" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
+      <c r="C201" s="15"/>
+      <c r="D201" s="15"/>
+    </row>
+    <row r="202" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B200" s="76">
-        <f>SUM(B185:B199)</f>
+      <c r="B202" s="76">
+        <f>SUM(B187:B201)</f>
         <v>0</v>
       </c>
-      <c r="C200" s="107" t="s">
+      <c r="C202" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D200" s="77"/>
-    </row>
-    <row r="201" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="78"/>
-      <c r="B201" s="78"/>
-      <c r="C201" s="78"/>
-      <c r="D201" s="78"/>
-    </row>
-    <row r="202" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="71" t="s">
+      <c r="D202" s="77"/>
+    </row>
+    <row r="203" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="78"/>
+      <c r="B203" s="78"/>
+      <c r="C203" s="78"/>
+      <c r="D203" s="78"/>
+    </row>
+    <row r="204" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B202" s="72">
+      <c r="B204" s="72">
         <v>15</v>
       </c>
-      <c r="C202" s="73" t="s">
+      <c r="C204" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D202" s="82">
+      <c r="D204" s="82">
         <v>42982</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="74" t="s">
+    <row r="205" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B203" s="75" t="s">
+      <c r="B205" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C203" s="74" t="s">
+      <c r="C205" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D203" s="74" t="s">
+      <c r="D205" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A204" s="9"/>
-      <c r="B204" s="8"/>
-      <c r="C204" s="13"/>
-      <c r="D204" s="13"/>
-    </row>
-    <row r="205" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A205" s="5"/>
-      <c r="B205" s="6"/>
-      <c r="C205" s="14"/>
-      <c r="D205" s="14"/>
-    </row>
     <row r="206" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A206" s="5"/>
-      <c r="B206" s="6"/>
-      <c r="C206" s="14"/>
-      <c r="D206" s="14"/>
+      <c r="A206" s="9"/>
+      <c r="B206" s="8"/>
+      <c r="C206" s="13"/>
+      <c r="D206" s="13"/>
     </row>
     <row r="207" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A207" s="5"/>
@@ -22400,13 +22508,13 @@
       <c r="D212" s="14"/>
     </row>
     <row r="213" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A213" s="6"/>
+      <c r="A213" s="5"/>
       <c r="B213" s="6"/>
       <c r="C213" s="14"/>
       <c r="D213" s="14"/>
     </row>
     <row r="214" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A214" s="6"/>
+      <c r="A214" s="5"/>
       <c r="B214" s="6"/>
       <c r="C214" s="14"/>
       <c r="D214" s="14"/>
@@ -22418,87 +22526,87 @@
       <c r="D215" s="14"/>
     </row>
     <row r="216" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A216" s="79"/>
-      <c r="B216" s="79"/>
-      <c r="C216" s="80"/>
-      <c r="D216" s="80"/>
+      <c r="A216" s="6"/>
+      <c r="B216" s="6"/>
+      <c r="C216" s="14"/>
+      <c r="D216" s="14"/>
     </row>
     <row r="217" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A217" s="79"/>
-      <c r="B217" s="79"/>
-      <c r="C217" s="80"/>
-      <c r="D217" s="80"/>
-    </row>
-    <row r="218" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="7"/>
-      <c r="B218" s="7"/>
-      <c r="C218" s="15"/>
-      <c r="D218" s="15"/>
-    </row>
-    <row r="219" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="76" t="s">
+      <c r="A217" s="6"/>
+      <c r="B217" s="6"/>
+      <c r="C217" s="14"/>
+      <c r="D217" s="14"/>
+    </row>
+    <row r="218" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A218" s="79"/>
+      <c r="B218" s="79"/>
+      <c r="C218" s="80"/>
+      <c r="D218" s="80"/>
+    </row>
+    <row r="219" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A219" s="79"/>
+      <c r="B219" s="79"/>
+      <c r="C219" s="80"/>
+      <c r="D219" s="80"/>
+    </row>
+    <row r="220" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="7"/>
+      <c r="B220" s="7"/>
+      <c r="C220" s="15"/>
+      <c r="D220" s="15"/>
+    </row>
+    <row r="221" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B219" s="76">
-        <f>SUM(B204:B218)</f>
+      <c r="B221" s="76">
+        <f>SUM(B206:B220)</f>
         <v>0</v>
       </c>
-      <c r="C219" s="107" t="s">
+      <c r="C221" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D219" s="77"/>
-    </row>
-    <row r="220" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="78"/>
-      <c r="B220" s="78"/>
-      <c r="C220" s="78"/>
-      <c r="D220" s="78"/>
-    </row>
-    <row r="221" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="71" t="s">
+      <c r="D221" s="77"/>
+    </row>
+    <row r="222" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A222" s="78"/>
+      <c r="B222" s="78"/>
+      <c r="C222" s="78"/>
+      <c r="D222" s="78"/>
+    </row>
+    <row r="223" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B221" s="72">
+      <c r="B223" s="72">
         <v>16</v>
       </c>
-      <c r="C221" s="73" t="s">
+      <c r="C223" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D221" s="82">
+      <c r="D223" s="82">
         <v>42989</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="74" t="s">
+    <row r="224" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B222" s="75" t="s">
+      <c r="B224" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C222" s="74" t="s">
+      <c r="C224" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D222" s="74" t="s">
+      <c r="D224" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A223" s="9"/>
-      <c r="B223" s="8"/>
-      <c r="C223" s="13"/>
-      <c r="D223" s="13"/>
-    </row>
-    <row r="224" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A224" s="5"/>
-      <c r="B224" s="6"/>
-      <c r="C224" s="14"/>
-      <c r="D224" s="14"/>
-    </row>
     <row r="225" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A225" s="5"/>
-      <c r="B225" s="6"/>
-      <c r="C225" s="14"/>
-      <c r="D225" s="14"/>
+      <c r="A225" s="9"/>
+      <c r="B225" s="8"/>
+      <c r="C225" s="13"/>
+      <c r="D225" s="13"/>
     </row>
     <row r="226" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A226" s="5"/>
@@ -22537,13 +22645,13 @@
       <c r="D231" s="14"/>
     </row>
     <row r="232" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A232" s="6"/>
+      <c r="A232" s="5"/>
       <c r="B232" s="6"/>
       <c r="C232" s="14"/>
       <c r="D232" s="14"/>
     </row>
     <row r="233" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A233" s="6"/>
+      <c r="A233" s="5"/>
       <c r="B233" s="6"/>
       <c r="C233" s="14"/>
       <c r="D233" s="14"/>
@@ -22555,57 +22663,69 @@
       <c r="D234" s="14"/>
     </row>
     <row r="235" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A235" s="79"/>
-      <c r="B235" s="79"/>
-      <c r="C235" s="80"/>
-      <c r="D235" s="80"/>
+      <c r="A235" s="6"/>
+      <c r="B235" s="6"/>
+      <c r="C235" s="14"/>
+      <c r="D235" s="14"/>
     </row>
     <row r="236" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A236" s="79"/>
-      <c r="B236" s="79"/>
-      <c r="C236" s="80"/>
-      <c r="D236" s="80"/>
-    </row>
-    <row r="237" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="7"/>
-      <c r="B237" s="7"/>
-      <c r="C237" s="15"/>
-      <c r="D237" s="15"/>
-    </row>
-    <row r="238" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="76" t="s">
+      <c r="A236" s="6"/>
+      <c r="B236" s="6"/>
+      <c r="C236" s="14"/>
+      <c r="D236" s="14"/>
+    </row>
+    <row r="237" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A237" s="79"/>
+      <c r="B237" s="79"/>
+      <c r="C237" s="80"/>
+      <c r="D237" s="80"/>
+    </row>
+    <row r="238" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A238" s="79"/>
+      <c r="B238" s="79"/>
+      <c r="C238" s="80"/>
+      <c r="D238" s="80"/>
+    </row>
+    <row r="239" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="7"/>
+      <c r="B239" s="7"/>
+      <c r="C239" s="15"/>
+      <c r="D239" s="15"/>
+    </row>
+    <row r="240" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B238" s="76">
-        <f>SUM(B223:B237)</f>
+      <c r="B240" s="76">
+        <f>SUM(B225:B239)</f>
         <v>0</v>
       </c>
-      <c r="C238" s="107" t="s">
+      <c r="C240" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D238" s="77"/>
-    </row>
-    <row r="239" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A239" s="78"/>
-      <c r="B239" s="78"/>
-      <c r="C239" s="78"/>
-      <c r="D239" s="78"/>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="106" t="s">
+      <c r="D240" s="77"/>
+    </row>
+    <row r="241" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A241" s="78"/>
+      <c r="B241" s="78"/>
+      <c r="C241" s="78"/>
+      <c r="D241" s="78"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="106" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F14 B71:B85 B90:B104 B109:B123 B128:B142 B147:B161 B166:B180 B185:B199 B204:B218 B223:B237 B61:B66 B51:B56 B42:B46 B31:B37 B20:B26 B9:B15 B3:B4">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F14 B71:B87 B92:B106 B111:B125 B130:B144 B149:B163 B168:B182 B187:B201 B206:B220 B225:B239 B61:B66 B51:B56 B42:B46 B31:B37 B20:B26 B9:B15 B3:B4">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B5 B16 B27 B38 B47 B57 B67 B86 B105 B124 B143 B162 B181 B200 B219 B238">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B5 B16 B27 B38 B47 B57 B67 B88 B107 B126 B145 B164 B183 B202 B221 B240">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A85 A90:A104 A109:A123 A128:A142 A147:A161 A166:A180 A185:A199 A204:A218 A223:A237 A61:A66 A51:A56 A42:A46 A31:A37 A20:A26 A9:A15 A3:A4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A87 A92:A106 A111:A125 A130:A144 A149:A163 A168:A182 A187:A201 A206:A220 A225:A239 A61:A66 A51:A56 A42:A46 A31:A37 A20:A26 A9:A15 A3:A4">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
MAJ JDT JLZ 14.06.2017
Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Doc/DemoMotJDT-Lopezji.xlsx
+++ b/Doc/DemoMotJDT-Lopezji.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="98">
   <si>
     <t>Module :</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>Design du site terminé. Tout le côté droit est rempli de personnages différents de jeux différents. Le côté gauche n'est une symétrie horizontale. (Si le temps le permet, le côté gauche sera aussi d'autres personnages différents)</t>
+  </si>
+  <si>
+    <t>J'ai cherché comment utiliser une extension créée. Après avoir suivi un tutoriel allemand avec beaucoup de difficultés, j'ai trouvé comment afficher le contenu de la table concernée par l'extension. Nous pouvons maintenant créer de nouvelles valeurs à partir du site directement mais il y a toujours un problème. Je n'arrive pas à insérer des données ou fichiers déjà existants. On peut uniquement en créer depuis le site. Je cherche avec Fabien comment on pourrait faire. On ne trouve pas donc on appelle Mme Hardegger pour nous aider. Elle nous indique qu'il manque une inclusion de l'extension dans le main template (inclure l'extension créée dans le template principal) mais cela n'a rien changé. Elle nous montre quel fichier il faut changer (Dans le dossier de l'extension se trouvent les fichiers de base comme les methodes utilisées pour afficher les différents contenus de la table concernée.) pour apporter des modifications à l'extension. Nous essayons donc d'abord de nous assurer que l'extension n'a besoin d'aucune modification via l'extension builder car une fois que nous modifions quelque chose directement via le code, il faut éviter d'effectuer une modification via le builder. Une fois l'extension confirmée j'ai essayé de modifié le code et maintenant je ne peux même plus créer de données depuis le frontend (site). J'essaye de nouvelles modification. J'ai ajouté un bouton "play" qui pour le moment fait afficher une page qui doit contenir les infos du jeu choisi (dans un future, cette page affichera un lien vers le jeu). Je fais un backup de l'extension pour si jamais. Je recréé une extension mais qui prend en compte l'utilisateur (car il faut savoir qui publie un jeu). La nouvelle extension contient deux tables (utilisateur et jeu). J'essaye de la mettre en place via la methode apprise mais le site affiche une erreur et rien ne s'affiche de plus. Peut-être lié au fait qu'il y ait deux tables avec une relation. J'essaye de supprimer une table pour confirmer mes doutes mais ça ne fonctionne pas. Je supprime donc l'extension qui, je crois ne fonctionne plus.</t>
+  </si>
+  <si>
+    <t>Mise à jour du journal de travail.</t>
   </si>
 </sst>
 </file>
@@ -1437,6 +1443,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1445,12 +1457,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3222,27 +3228,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3272,27 +3278,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3330,470 +3336,470 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="110" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="114"/>
+      <c r="AE2" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="111"/>
-      <c r="AG2" s="111"/>
-      <c r="AH2" s="111"/>
-      <c r="AI2" s="111"/>
-      <c r="AJ2" s="111"/>
-      <c r="AK2" s="111"/>
-      <c r="AL2" s="111"/>
-      <c r="AM2" s="111"/>
-      <c r="AN2" s="111"/>
-      <c r="AO2" s="111"/>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="111"/>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AU2" s="111"/>
-      <c r="AV2" s="111"/>
-      <c r="AW2" s="111"/>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="111"/>
-      <c r="AZ2" s="111"/>
-      <c r="BA2" s="111"/>
-      <c r="BB2" s="111"/>
-      <c r="BC2" s="111"/>
-      <c r="BD2" s="111"/>
-      <c r="BE2" s="112"/>
-      <c r="BF2" s="110" t="s">
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AH2" s="113"/>
+      <c r="AI2" s="113"/>
+      <c r="AJ2" s="113"/>
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="113"/>
+      <c r="AO2" s="113"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="113"/>
+      <c r="AR2" s="113"/>
+      <c r="AS2" s="113"/>
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BD2" s="113"/>
+      <c r="BE2" s="114"/>
+      <c r="BF2" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="BG2" s="111"/>
-      <c r="BH2" s="111"/>
-      <c r="BI2" s="111"/>
-      <c r="BJ2" s="111"/>
-      <c r="BK2" s="111"/>
-      <c r="BL2" s="111"/>
-      <c r="BM2" s="111"/>
-      <c r="BN2" s="111"/>
-      <c r="BO2" s="111"/>
-      <c r="BP2" s="111"/>
-      <c r="BQ2" s="111"/>
-      <c r="BR2" s="111"/>
-      <c r="BS2" s="111"/>
-      <c r="BT2" s="111"/>
-      <c r="BU2" s="111"/>
-      <c r="BV2" s="111"/>
-      <c r="BW2" s="111"/>
-      <c r="BX2" s="111"/>
-      <c r="BY2" s="111"/>
-      <c r="BZ2" s="111"/>
-      <c r="CA2" s="111"/>
-      <c r="CB2" s="111"/>
-      <c r="CC2" s="111"/>
-      <c r="CD2" s="111"/>
-      <c r="CE2" s="111"/>
-      <c r="CF2" s="112"/>
-      <c r="CG2" s="110" t="s">
+      <c r="BG2" s="113"/>
+      <c r="BH2" s="113"/>
+      <c r="BI2" s="113"/>
+      <c r="BJ2" s="113"/>
+      <c r="BK2" s="113"/>
+      <c r="BL2" s="113"/>
+      <c r="BM2" s="113"/>
+      <c r="BN2" s="113"/>
+      <c r="BO2" s="113"/>
+      <c r="BP2" s="113"/>
+      <c r="BQ2" s="113"/>
+      <c r="BR2" s="113"/>
+      <c r="BS2" s="113"/>
+      <c r="BT2" s="113"/>
+      <c r="BU2" s="113"/>
+      <c r="BV2" s="113"/>
+      <c r="BW2" s="113"/>
+      <c r="BX2" s="113"/>
+      <c r="BY2" s="113"/>
+      <c r="BZ2" s="113"/>
+      <c r="CA2" s="113"/>
+      <c r="CB2" s="113"/>
+      <c r="CC2" s="113"/>
+      <c r="CD2" s="113"/>
+      <c r="CE2" s="113"/>
+      <c r="CF2" s="114"/>
+      <c r="CG2" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="CH2" s="111"/>
-      <c r="CI2" s="111"/>
-      <c r="CJ2" s="111"/>
-      <c r="CK2" s="111"/>
-      <c r="CL2" s="111"/>
-      <c r="CM2" s="111"/>
-      <c r="CN2" s="111"/>
-      <c r="CO2" s="111"/>
-      <c r="CP2" s="111"/>
-      <c r="CQ2" s="111"/>
-      <c r="CR2" s="111"/>
-      <c r="CS2" s="111"/>
-      <c r="CT2" s="111"/>
-      <c r="CU2" s="111"/>
-      <c r="CV2" s="111"/>
-      <c r="CW2" s="111"/>
-      <c r="CX2" s="111"/>
-      <c r="CY2" s="111"/>
-      <c r="CZ2" s="111"/>
-      <c r="DA2" s="111"/>
-      <c r="DB2" s="111"/>
-      <c r="DC2" s="111"/>
-      <c r="DD2" s="111"/>
-      <c r="DE2" s="111"/>
-      <c r="DF2" s="111"/>
-      <c r="DG2" s="112"/>
-      <c r="DH2" s="110" t="s">
+      <c r="CH2" s="113"/>
+      <c r="CI2" s="113"/>
+      <c r="CJ2" s="113"/>
+      <c r="CK2" s="113"/>
+      <c r="CL2" s="113"/>
+      <c r="CM2" s="113"/>
+      <c r="CN2" s="113"/>
+      <c r="CO2" s="113"/>
+      <c r="CP2" s="113"/>
+      <c r="CQ2" s="113"/>
+      <c r="CR2" s="113"/>
+      <c r="CS2" s="113"/>
+      <c r="CT2" s="113"/>
+      <c r="CU2" s="113"/>
+      <c r="CV2" s="113"/>
+      <c r="CW2" s="113"/>
+      <c r="CX2" s="113"/>
+      <c r="CY2" s="113"/>
+      <c r="CZ2" s="113"/>
+      <c r="DA2" s="113"/>
+      <c r="DB2" s="113"/>
+      <c r="DC2" s="113"/>
+      <c r="DD2" s="113"/>
+      <c r="DE2" s="113"/>
+      <c r="DF2" s="113"/>
+      <c r="DG2" s="114"/>
+      <c r="DH2" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="DI2" s="111"/>
-      <c r="DJ2" s="111"/>
-      <c r="DK2" s="111"/>
-      <c r="DL2" s="111"/>
-      <c r="DM2" s="111"/>
-      <c r="DN2" s="111"/>
-      <c r="DO2" s="111"/>
-      <c r="DP2" s="111"/>
-      <c r="DQ2" s="111"/>
-      <c r="DR2" s="111"/>
-      <c r="DS2" s="111"/>
-      <c r="DT2" s="111"/>
-      <c r="DU2" s="111"/>
-      <c r="DV2" s="111"/>
-      <c r="DW2" s="111"/>
-      <c r="DX2" s="111"/>
-      <c r="DY2" s="111"/>
-      <c r="DZ2" s="111"/>
-      <c r="EA2" s="111"/>
-      <c r="EB2" s="111"/>
-      <c r="EC2" s="111"/>
-      <c r="ED2" s="111"/>
-      <c r="EE2" s="111"/>
-      <c r="EF2" s="111"/>
-      <c r="EG2" s="111"/>
-      <c r="EH2" s="112"/>
-      <c r="EI2" s="110" t="s">
+      <c r="DI2" s="113"/>
+      <c r="DJ2" s="113"/>
+      <c r="DK2" s="113"/>
+      <c r="DL2" s="113"/>
+      <c r="DM2" s="113"/>
+      <c r="DN2" s="113"/>
+      <c r="DO2" s="113"/>
+      <c r="DP2" s="113"/>
+      <c r="DQ2" s="113"/>
+      <c r="DR2" s="113"/>
+      <c r="DS2" s="113"/>
+      <c r="DT2" s="113"/>
+      <c r="DU2" s="113"/>
+      <c r="DV2" s="113"/>
+      <c r="DW2" s="113"/>
+      <c r="DX2" s="113"/>
+      <c r="DY2" s="113"/>
+      <c r="DZ2" s="113"/>
+      <c r="EA2" s="113"/>
+      <c r="EB2" s="113"/>
+      <c r="EC2" s="113"/>
+      <c r="ED2" s="113"/>
+      <c r="EE2" s="113"/>
+      <c r="EF2" s="113"/>
+      <c r="EG2" s="113"/>
+      <c r="EH2" s="114"/>
+      <c r="EI2" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="111"/>
-      <c r="EK2" s="111"/>
-      <c r="EL2" s="111"/>
-      <c r="EM2" s="111"/>
-      <c r="EN2" s="111"/>
-      <c r="EO2" s="111"/>
-      <c r="EP2" s="111"/>
-      <c r="EQ2" s="111"/>
-      <c r="ER2" s="111"/>
-      <c r="ES2" s="111"/>
-      <c r="ET2" s="111"/>
-      <c r="EU2" s="111"/>
-      <c r="EV2" s="111"/>
-      <c r="EW2" s="111"/>
-      <c r="EX2" s="111"/>
-      <c r="EY2" s="111"/>
-      <c r="EZ2" s="111"/>
-      <c r="FA2" s="111"/>
-      <c r="FB2" s="111"/>
-      <c r="FC2" s="111"/>
-      <c r="FD2" s="111"/>
-      <c r="FE2" s="111"/>
-      <c r="FF2" s="111"/>
-      <c r="FG2" s="111"/>
-      <c r="FH2" s="111"/>
-      <c r="FI2" s="112"/>
-      <c r="FJ2" s="110" t="s">
+      <c r="EJ2" s="113"/>
+      <c r="EK2" s="113"/>
+      <c r="EL2" s="113"/>
+      <c r="EM2" s="113"/>
+      <c r="EN2" s="113"/>
+      <c r="EO2" s="113"/>
+      <c r="EP2" s="113"/>
+      <c r="EQ2" s="113"/>
+      <c r="ER2" s="113"/>
+      <c r="ES2" s="113"/>
+      <c r="ET2" s="113"/>
+      <c r="EU2" s="113"/>
+      <c r="EV2" s="113"/>
+      <c r="EW2" s="113"/>
+      <c r="EX2" s="113"/>
+      <c r="EY2" s="113"/>
+      <c r="EZ2" s="113"/>
+      <c r="FA2" s="113"/>
+      <c r="FB2" s="113"/>
+      <c r="FC2" s="113"/>
+      <c r="FD2" s="113"/>
+      <c r="FE2" s="113"/>
+      <c r="FF2" s="113"/>
+      <c r="FG2" s="113"/>
+      <c r="FH2" s="113"/>
+      <c r="FI2" s="114"/>
+      <c r="FJ2" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="FK2" s="111"/>
-      <c r="FL2" s="111"/>
-      <c r="FM2" s="111"/>
-      <c r="FN2" s="111"/>
-      <c r="FO2" s="111"/>
-      <c r="FP2" s="111"/>
-      <c r="FQ2" s="111"/>
-      <c r="FR2" s="111"/>
-      <c r="FS2" s="111"/>
-      <c r="FT2" s="111"/>
-      <c r="FU2" s="111"/>
-      <c r="FV2" s="111"/>
-      <c r="FW2" s="111"/>
-      <c r="FX2" s="111"/>
-      <c r="FY2" s="111"/>
-      <c r="FZ2" s="111"/>
-      <c r="GA2" s="111"/>
-      <c r="GB2" s="111"/>
-      <c r="GC2" s="111"/>
-      <c r="GD2" s="111"/>
-      <c r="GE2" s="111"/>
-      <c r="GF2" s="111"/>
-      <c r="GG2" s="111"/>
-      <c r="GH2" s="111"/>
-      <c r="GI2" s="111"/>
-      <c r="GJ2" s="112"/>
-      <c r="GK2" s="110" t="s">
+      <c r="FK2" s="113"/>
+      <c r="FL2" s="113"/>
+      <c r="FM2" s="113"/>
+      <c r="FN2" s="113"/>
+      <c r="FO2" s="113"/>
+      <c r="FP2" s="113"/>
+      <c r="FQ2" s="113"/>
+      <c r="FR2" s="113"/>
+      <c r="FS2" s="113"/>
+      <c r="FT2" s="113"/>
+      <c r="FU2" s="113"/>
+      <c r="FV2" s="113"/>
+      <c r="FW2" s="113"/>
+      <c r="FX2" s="113"/>
+      <c r="FY2" s="113"/>
+      <c r="FZ2" s="113"/>
+      <c r="GA2" s="113"/>
+      <c r="GB2" s="113"/>
+      <c r="GC2" s="113"/>
+      <c r="GD2" s="113"/>
+      <c r="GE2" s="113"/>
+      <c r="GF2" s="113"/>
+      <c r="GG2" s="113"/>
+      <c r="GH2" s="113"/>
+      <c r="GI2" s="113"/>
+      <c r="GJ2" s="114"/>
+      <c r="GK2" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="GL2" s="111"/>
-      <c r="GM2" s="111"/>
-      <c r="GN2" s="111"/>
-      <c r="GO2" s="111"/>
-      <c r="GP2" s="111"/>
-      <c r="GQ2" s="111"/>
-      <c r="GR2" s="111"/>
-      <c r="GS2" s="111"/>
-      <c r="GT2" s="111"/>
-      <c r="GU2" s="111"/>
-      <c r="GV2" s="111"/>
-      <c r="GW2" s="111"/>
-      <c r="GX2" s="111"/>
-      <c r="GY2" s="111"/>
-      <c r="GZ2" s="111"/>
-      <c r="HA2" s="111"/>
-      <c r="HB2" s="111"/>
-      <c r="HC2" s="111"/>
-      <c r="HD2" s="111"/>
-      <c r="HE2" s="111"/>
-      <c r="HF2" s="111"/>
-      <c r="HG2" s="111"/>
-      <c r="HH2" s="111"/>
-      <c r="HI2" s="111"/>
-      <c r="HJ2" s="111"/>
-      <c r="HK2" s="112"/>
-      <c r="HL2" s="110" t="s">
+      <c r="GL2" s="113"/>
+      <c r="GM2" s="113"/>
+      <c r="GN2" s="113"/>
+      <c r="GO2" s="113"/>
+      <c r="GP2" s="113"/>
+      <c r="GQ2" s="113"/>
+      <c r="GR2" s="113"/>
+      <c r="GS2" s="113"/>
+      <c r="GT2" s="113"/>
+      <c r="GU2" s="113"/>
+      <c r="GV2" s="113"/>
+      <c r="GW2" s="113"/>
+      <c r="GX2" s="113"/>
+      <c r="GY2" s="113"/>
+      <c r="GZ2" s="113"/>
+      <c r="HA2" s="113"/>
+      <c r="HB2" s="113"/>
+      <c r="HC2" s="113"/>
+      <c r="HD2" s="113"/>
+      <c r="HE2" s="113"/>
+      <c r="HF2" s="113"/>
+      <c r="HG2" s="113"/>
+      <c r="HH2" s="113"/>
+      <c r="HI2" s="113"/>
+      <c r="HJ2" s="113"/>
+      <c r="HK2" s="114"/>
+      <c r="HL2" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="HM2" s="111"/>
-      <c r="HN2" s="111"/>
-      <c r="HO2" s="111"/>
-      <c r="HP2" s="111"/>
-      <c r="HQ2" s="111"/>
-      <c r="HR2" s="111"/>
-      <c r="HS2" s="111"/>
-      <c r="HT2" s="111"/>
-      <c r="HU2" s="111"/>
-      <c r="HV2" s="111"/>
-      <c r="HW2" s="111"/>
-      <c r="HX2" s="111"/>
-      <c r="HY2" s="111"/>
-      <c r="HZ2" s="111"/>
-      <c r="IA2" s="111"/>
-      <c r="IB2" s="111"/>
-      <c r="IC2" s="111"/>
-      <c r="ID2" s="111"/>
-      <c r="IE2" s="111"/>
-      <c r="IF2" s="111"/>
-      <c r="IG2" s="111"/>
-      <c r="IH2" s="111"/>
-      <c r="II2" s="111"/>
-      <c r="IJ2" s="111"/>
-      <c r="IK2" s="111"/>
-      <c r="IL2" s="112"/>
-      <c r="IM2" s="110" t="s">
+      <c r="HM2" s="113"/>
+      <c r="HN2" s="113"/>
+      <c r="HO2" s="113"/>
+      <c r="HP2" s="113"/>
+      <c r="HQ2" s="113"/>
+      <c r="HR2" s="113"/>
+      <c r="HS2" s="113"/>
+      <c r="HT2" s="113"/>
+      <c r="HU2" s="113"/>
+      <c r="HV2" s="113"/>
+      <c r="HW2" s="113"/>
+      <c r="HX2" s="113"/>
+      <c r="HY2" s="113"/>
+      <c r="HZ2" s="113"/>
+      <c r="IA2" s="113"/>
+      <c r="IB2" s="113"/>
+      <c r="IC2" s="113"/>
+      <c r="ID2" s="113"/>
+      <c r="IE2" s="113"/>
+      <c r="IF2" s="113"/>
+      <c r="IG2" s="113"/>
+      <c r="IH2" s="113"/>
+      <c r="II2" s="113"/>
+      <c r="IJ2" s="113"/>
+      <c r="IK2" s="113"/>
+      <c r="IL2" s="114"/>
+      <c r="IM2" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="IN2" s="111"/>
-      <c r="IO2" s="111"/>
-      <c r="IP2" s="111"/>
-      <c r="IQ2" s="111"/>
-      <c r="IR2" s="111"/>
-      <c r="IS2" s="111"/>
-      <c r="IT2" s="111"/>
-      <c r="IU2" s="111"/>
-      <c r="IV2" s="111"/>
-      <c r="IW2" s="111"/>
-      <c r="IX2" s="111"/>
-      <c r="IY2" s="111"/>
-      <c r="IZ2" s="111"/>
-      <c r="JA2" s="111"/>
-      <c r="JB2" s="111"/>
-      <c r="JC2" s="111"/>
-      <c r="JD2" s="111"/>
-      <c r="JE2" s="111"/>
-      <c r="JF2" s="111"/>
-      <c r="JG2" s="111"/>
-      <c r="JH2" s="111"/>
-      <c r="JI2" s="111"/>
-      <c r="JJ2" s="111"/>
-      <c r="JK2" s="111"/>
-      <c r="JL2" s="111"/>
-      <c r="JM2" s="112"/>
-      <c r="JN2" s="110" t="s">
+      <c r="IN2" s="113"/>
+      <c r="IO2" s="113"/>
+      <c r="IP2" s="113"/>
+      <c r="IQ2" s="113"/>
+      <c r="IR2" s="113"/>
+      <c r="IS2" s="113"/>
+      <c r="IT2" s="113"/>
+      <c r="IU2" s="113"/>
+      <c r="IV2" s="113"/>
+      <c r="IW2" s="113"/>
+      <c r="IX2" s="113"/>
+      <c r="IY2" s="113"/>
+      <c r="IZ2" s="113"/>
+      <c r="JA2" s="113"/>
+      <c r="JB2" s="113"/>
+      <c r="JC2" s="113"/>
+      <c r="JD2" s="113"/>
+      <c r="JE2" s="113"/>
+      <c r="JF2" s="113"/>
+      <c r="JG2" s="113"/>
+      <c r="JH2" s="113"/>
+      <c r="JI2" s="113"/>
+      <c r="JJ2" s="113"/>
+      <c r="JK2" s="113"/>
+      <c r="JL2" s="113"/>
+      <c r="JM2" s="114"/>
+      <c r="JN2" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="JO2" s="111"/>
-      <c r="JP2" s="111"/>
-      <c r="JQ2" s="111"/>
-      <c r="JR2" s="111"/>
-      <c r="JS2" s="111"/>
-      <c r="JT2" s="111"/>
-      <c r="JU2" s="111"/>
-      <c r="JV2" s="111"/>
-      <c r="JW2" s="111"/>
-      <c r="JX2" s="111"/>
-      <c r="JY2" s="111"/>
-      <c r="JZ2" s="111"/>
-      <c r="KA2" s="111"/>
-      <c r="KB2" s="111"/>
-      <c r="KC2" s="111"/>
-      <c r="KD2" s="111"/>
-      <c r="KE2" s="111"/>
-      <c r="KF2" s="111"/>
-      <c r="KG2" s="111"/>
-      <c r="KH2" s="111"/>
-      <c r="KI2" s="111"/>
-      <c r="KJ2" s="111"/>
-      <c r="KK2" s="111"/>
-      <c r="KL2" s="111"/>
-      <c r="KM2" s="111"/>
-      <c r="KN2" s="112"/>
-      <c r="KO2" s="110" t="s">
+      <c r="JO2" s="113"/>
+      <c r="JP2" s="113"/>
+      <c r="JQ2" s="113"/>
+      <c r="JR2" s="113"/>
+      <c r="JS2" s="113"/>
+      <c r="JT2" s="113"/>
+      <c r="JU2" s="113"/>
+      <c r="JV2" s="113"/>
+      <c r="JW2" s="113"/>
+      <c r="JX2" s="113"/>
+      <c r="JY2" s="113"/>
+      <c r="JZ2" s="113"/>
+      <c r="KA2" s="113"/>
+      <c r="KB2" s="113"/>
+      <c r="KC2" s="113"/>
+      <c r="KD2" s="113"/>
+      <c r="KE2" s="113"/>
+      <c r="KF2" s="113"/>
+      <c r="KG2" s="113"/>
+      <c r="KH2" s="113"/>
+      <c r="KI2" s="113"/>
+      <c r="KJ2" s="113"/>
+      <c r="KK2" s="113"/>
+      <c r="KL2" s="113"/>
+      <c r="KM2" s="113"/>
+      <c r="KN2" s="114"/>
+      <c r="KO2" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="KP2" s="111"/>
-      <c r="KQ2" s="111"/>
-      <c r="KR2" s="111"/>
-      <c r="KS2" s="111"/>
-      <c r="KT2" s="111"/>
-      <c r="KU2" s="111"/>
-      <c r="KV2" s="111"/>
-      <c r="KW2" s="111"/>
-      <c r="KX2" s="111"/>
-      <c r="KY2" s="111"/>
-      <c r="KZ2" s="111"/>
-      <c r="LA2" s="111"/>
-      <c r="LB2" s="111"/>
-      <c r="LC2" s="111"/>
-      <c r="LD2" s="111"/>
-      <c r="LE2" s="111"/>
-      <c r="LF2" s="111"/>
-      <c r="LG2" s="111"/>
-      <c r="LH2" s="111"/>
-      <c r="LI2" s="111"/>
-      <c r="LJ2" s="111"/>
-      <c r="LK2" s="111"/>
-      <c r="LL2" s="111"/>
-      <c r="LM2" s="111"/>
-      <c r="LN2" s="111"/>
-      <c r="LO2" s="112"/>
-      <c r="LP2" s="110" t="s">
+      <c r="KP2" s="113"/>
+      <c r="KQ2" s="113"/>
+      <c r="KR2" s="113"/>
+      <c r="KS2" s="113"/>
+      <c r="KT2" s="113"/>
+      <c r="KU2" s="113"/>
+      <c r="KV2" s="113"/>
+      <c r="KW2" s="113"/>
+      <c r="KX2" s="113"/>
+      <c r="KY2" s="113"/>
+      <c r="KZ2" s="113"/>
+      <c r="LA2" s="113"/>
+      <c r="LB2" s="113"/>
+      <c r="LC2" s="113"/>
+      <c r="LD2" s="113"/>
+      <c r="LE2" s="113"/>
+      <c r="LF2" s="113"/>
+      <c r="LG2" s="113"/>
+      <c r="LH2" s="113"/>
+      <c r="LI2" s="113"/>
+      <c r="LJ2" s="113"/>
+      <c r="LK2" s="113"/>
+      <c r="LL2" s="113"/>
+      <c r="LM2" s="113"/>
+      <c r="LN2" s="113"/>
+      <c r="LO2" s="114"/>
+      <c r="LP2" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="LQ2" s="111"/>
-      <c r="LR2" s="111"/>
-      <c r="LS2" s="111"/>
-      <c r="LT2" s="111"/>
-      <c r="LU2" s="111"/>
-      <c r="LV2" s="111"/>
-      <c r="LW2" s="111"/>
-      <c r="LX2" s="111"/>
-      <c r="LY2" s="111"/>
-      <c r="LZ2" s="111"/>
-      <c r="MA2" s="111"/>
-      <c r="MB2" s="111"/>
-      <c r="MC2" s="111"/>
-      <c r="MD2" s="111"/>
-      <c r="ME2" s="111"/>
-      <c r="MF2" s="111"/>
-      <c r="MG2" s="111"/>
-      <c r="MH2" s="111"/>
-      <c r="MI2" s="111"/>
-      <c r="MJ2" s="111"/>
-      <c r="MK2" s="111"/>
-      <c r="ML2" s="111"/>
-      <c r="MM2" s="111"/>
-      <c r="MN2" s="111"/>
-      <c r="MO2" s="111"/>
-      <c r="MP2" s="112"/>
-      <c r="MQ2" s="110" t="s">
+      <c r="LQ2" s="113"/>
+      <c r="LR2" s="113"/>
+      <c r="LS2" s="113"/>
+      <c r="LT2" s="113"/>
+      <c r="LU2" s="113"/>
+      <c r="LV2" s="113"/>
+      <c r="LW2" s="113"/>
+      <c r="LX2" s="113"/>
+      <c r="LY2" s="113"/>
+      <c r="LZ2" s="113"/>
+      <c r="MA2" s="113"/>
+      <c r="MB2" s="113"/>
+      <c r="MC2" s="113"/>
+      <c r="MD2" s="113"/>
+      <c r="ME2" s="113"/>
+      <c r="MF2" s="113"/>
+      <c r="MG2" s="113"/>
+      <c r="MH2" s="113"/>
+      <c r="MI2" s="113"/>
+      <c r="MJ2" s="113"/>
+      <c r="MK2" s="113"/>
+      <c r="ML2" s="113"/>
+      <c r="MM2" s="113"/>
+      <c r="MN2" s="113"/>
+      <c r="MO2" s="113"/>
+      <c r="MP2" s="114"/>
+      <c r="MQ2" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="MR2" s="111"/>
-      <c r="MS2" s="111"/>
-      <c r="MT2" s="111"/>
-      <c r="MU2" s="111"/>
-      <c r="MV2" s="111"/>
-      <c r="MW2" s="111"/>
-      <c r="MX2" s="111"/>
-      <c r="MY2" s="111"/>
-      <c r="MZ2" s="111"/>
-      <c r="NA2" s="111"/>
-      <c r="NB2" s="111"/>
-      <c r="NC2" s="111"/>
-      <c r="ND2" s="111"/>
-      <c r="NE2" s="111"/>
-      <c r="NF2" s="111"/>
-      <c r="NG2" s="111"/>
-      <c r="NH2" s="111"/>
-      <c r="NI2" s="111"/>
-      <c r="NJ2" s="111"/>
-      <c r="NK2" s="111"/>
-      <c r="NL2" s="111"/>
-      <c r="NM2" s="111"/>
-      <c r="NN2" s="111"/>
-      <c r="NO2" s="111"/>
-      <c r="NP2" s="111"/>
-      <c r="NQ2" s="112"/>
-      <c r="NR2" s="110" t="s">
+      <c r="MR2" s="113"/>
+      <c r="MS2" s="113"/>
+      <c r="MT2" s="113"/>
+      <c r="MU2" s="113"/>
+      <c r="MV2" s="113"/>
+      <c r="MW2" s="113"/>
+      <c r="MX2" s="113"/>
+      <c r="MY2" s="113"/>
+      <c r="MZ2" s="113"/>
+      <c r="NA2" s="113"/>
+      <c r="NB2" s="113"/>
+      <c r="NC2" s="113"/>
+      <c r="ND2" s="113"/>
+      <c r="NE2" s="113"/>
+      <c r="NF2" s="113"/>
+      <c r="NG2" s="113"/>
+      <c r="NH2" s="113"/>
+      <c r="NI2" s="113"/>
+      <c r="NJ2" s="113"/>
+      <c r="NK2" s="113"/>
+      <c r="NL2" s="113"/>
+      <c r="NM2" s="113"/>
+      <c r="NN2" s="113"/>
+      <c r="NO2" s="113"/>
+      <c r="NP2" s="113"/>
+      <c r="NQ2" s="114"/>
+      <c r="NR2" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="NS2" s="111"/>
-      <c r="NT2" s="111"/>
-      <c r="NU2" s="111"/>
-      <c r="NV2" s="111"/>
-      <c r="NW2" s="111"/>
-      <c r="NX2" s="111"/>
-      <c r="NY2" s="111"/>
-      <c r="NZ2" s="111"/>
-      <c r="OA2" s="111"/>
-      <c r="OB2" s="111"/>
-      <c r="OC2" s="111"/>
-      <c r="OD2" s="111"/>
-      <c r="OE2" s="111"/>
-      <c r="OF2" s="111"/>
-      <c r="OG2" s="111"/>
-      <c r="OH2" s="111"/>
-      <c r="OI2" s="111"/>
-      <c r="OJ2" s="111"/>
-      <c r="OK2" s="111"/>
-      <c r="OL2" s="111"/>
-      <c r="OM2" s="111"/>
-      <c r="ON2" s="111"/>
-      <c r="OO2" s="111"/>
-      <c r="OP2" s="111"/>
-      <c r="OQ2" s="111"/>
-      <c r="OR2" s="112"/>
-      <c r="OS2" s="110" t="s">
+      <c r="NS2" s="113"/>
+      <c r="NT2" s="113"/>
+      <c r="NU2" s="113"/>
+      <c r="NV2" s="113"/>
+      <c r="NW2" s="113"/>
+      <c r="NX2" s="113"/>
+      <c r="NY2" s="113"/>
+      <c r="NZ2" s="113"/>
+      <c r="OA2" s="113"/>
+      <c r="OB2" s="113"/>
+      <c r="OC2" s="113"/>
+      <c r="OD2" s="113"/>
+      <c r="OE2" s="113"/>
+      <c r="OF2" s="113"/>
+      <c r="OG2" s="113"/>
+      <c r="OH2" s="113"/>
+      <c r="OI2" s="113"/>
+      <c r="OJ2" s="113"/>
+      <c r="OK2" s="113"/>
+      <c r="OL2" s="113"/>
+      <c r="OM2" s="113"/>
+      <c r="ON2" s="113"/>
+      <c r="OO2" s="113"/>
+      <c r="OP2" s="113"/>
+      <c r="OQ2" s="113"/>
+      <c r="OR2" s="114"/>
+      <c r="OS2" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="OT2" s="111"/>
-      <c r="OU2" s="111"/>
-      <c r="OV2" s="111"/>
-      <c r="OW2" s="111"/>
-      <c r="OX2" s="111"/>
-      <c r="OY2" s="111"/>
-      <c r="OZ2" s="111"/>
-      <c r="PA2" s="111"/>
-      <c r="PB2" s="111"/>
-      <c r="PC2" s="111"/>
-      <c r="PD2" s="111"/>
-      <c r="PE2" s="111"/>
-      <c r="PF2" s="111"/>
-      <c r="PG2" s="111"/>
-      <c r="PH2" s="111"/>
-      <c r="PI2" s="111"/>
-      <c r="PJ2" s="111"/>
-      <c r="PK2" s="111"/>
-      <c r="PL2" s="111"/>
-      <c r="PM2" s="111"/>
-      <c r="PN2" s="111"/>
-      <c r="PO2" s="111"/>
-      <c r="PP2" s="111"/>
-      <c r="PQ2" s="111"/>
-      <c r="PR2" s="111"/>
-      <c r="PS2" s="112"/>
+      <c r="OT2" s="113"/>
+      <c r="OU2" s="113"/>
+      <c r="OV2" s="113"/>
+      <c r="OW2" s="113"/>
+      <c r="OX2" s="113"/>
+      <c r="OY2" s="113"/>
+      <c r="OZ2" s="113"/>
+      <c r="PA2" s="113"/>
+      <c r="PB2" s="113"/>
+      <c r="PC2" s="113"/>
+      <c r="PD2" s="113"/>
+      <c r="PE2" s="113"/>
+      <c r="PF2" s="113"/>
+      <c r="PG2" s="113"/>
+      <c r="PH2" s="113"/>
+      <c r="PI2" s="113"/>
+      <c r="PJ2" s="113"/>
+      <c r="PK2" s="113"/>
+      <c r="PL2" s="113"/>
+      <c r="PM2" s="113"/>
+      <c r="PN2" s="113"/>
+      <c r="PO2" s="113"/>
+      <c r="PP2" s="113"/>
+      <c r="PQ2" s="113"/>
+      <c r="PR2" s="113"/>
+      <c r="PS2" s="114"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
@@ -5117,7 +5123,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="114"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5555,7 +5561,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="113" t="str">
+      <c r="B7" s="110" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -5996,7 +6002,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="114"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6434,7 +6440,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="113" t="str">
+      <c r="B9" s="110" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -6875,7 +6881,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="114"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7313,7 +7319,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="113" t="str">
+      <c r="B11" s="110" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7754,7 +7760,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="114"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8192,7 +8198,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="113" t="str">
+      <c r="B13" s="110" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8633,7 +8639,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="114"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -9071,7 +9077,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="113" t="str">
+      <c r="B15" s="110" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9513,7 +9519,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="114"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -9951,7 +9957,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="113" t="str">
+      <c r="B17" s="110" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10392,7 +10398,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="114"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -10830,7 +10836,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="113" t="str">
+      <c r="B19" s="110" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11271,7 +11277,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="114"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11709,7 +11715,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="113" t="str">
+      <c r="B21" s="110" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12150,7 +12156,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="114"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12588,7 +12594,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="113" t="str">
+      <c r="B23" s="110" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -13029,7 +13035,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="114"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13467,7 +13473,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="113" t="str">
+      <c r="B25" s="110" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -13908,7 +13914,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="114"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14346,7 +14352,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="113" t="str">
+      <c r="B27" s="110" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -14787,7 +14793,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="114"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15225,7 +15231,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="113" t="str">
+      <c r="B29" s="110" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15666,7 +15672,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="114"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16104,7 +16110,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="113" t="str">
+      <c r="B31" s="110" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16545,7 +16551,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="114"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -17867,14 +17873,13 @@
   </sheetData>
   <sheetProtection insertRows="0" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="HL2:IL2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="CG2:DG2"/>
-    <mergeCell ref="DH2:EH2"/>
-    <mergeCell ref="EI2:FI2"/>
-    <mergeCell ref="FJ2:GJ2"/>
-    <mergeCell ref="GK2:HK2"/>
+    <mergeCell ref="OS2:PS2"/>
+    <mergeCell ref="IM2:JM2"/>
+    <mergeCell ref="JN2:KN2"/>
+    <mergeCell ref="KO2:LO2"/>
+    <mergeCell ref="LP2:MP2"/>
+    <mergeCell ref="MQ2:NQ2"/>
+    <mergeCell ref="NR2:OR2"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="D2:AD2"/>
@@ -17891,13 +17896,14 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="OS2:PS2"/>
-    <mergeCell ref="IM2:JM2"/>
-    <mergeCell ref="JN2:KN2"/>
-    <mergeCell ref="KO2:LO2"/>
-    <mergeCell ref="LP2:MP2"/>
-    <mergeCell ref="MQ2:NQ2"/>
-    <mergeCell ref="NR2:OR2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="HL2:IL2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="CG2:DG2"/>
+    <mergeCell ref="DH2:EH2"/>
+    <mergeCell ref="EI2:FI2"/>
+    <mergeCell ref="FJ2:GJ2"/>
+    <mergeCell ref="GK2:HK2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C33">
@@ -20568,8 +20574,8 @@
   </sheetPr>
   <dimension ref="A1:I242"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A88" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A109" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21763,7 +21769,7 @@
         <v>23</v>
       </c>
       <c r="D109" s="82">
-        <v>42947</v>
+        <v>42901</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -21781,27 +21787,51 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A111" s="9"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="13"/>
+      <c r="A111" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B111" s="8">
+        <v>1</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="D111" s="13"/>
     </row>
-    <row r="112" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A112" s="5"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="14"/>
+    <row r="112" spans="1:4" ht="324" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B112" s="6">
+        <v>24</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="D112" s="14"/>
     </row>
     <row r="113" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
-      <c r="B113" s="6"/>
-      <c r="C113" s="14"/>
+      <c r="A113" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B113" s="6">
+        <v>1</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="D113" s="14"/>
     </row>
     <row r="114" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="5"/>
-      <c r="B114" s="6"/>
-      <c r="C114" s="14"/>
+      <c r="A114" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114" s="6">
+        <v>1</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="D114" s="14"/>
     </row>
     <row r="115" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -21876,7 +21906,7 @@
       </c>
       <c r="B126" s="76">
         <f>SUM(B111:B125)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C126" s="107" t="s">
         <v>44</v>

</xml_diff>